<commit_message>
Unfiltered output written to separate subdirectory; duplicate filter_deadband logic removed
</commit_message>
<xml_diff>
--- a/data-raw/skyline_meta-data.xlsx
+++ b/data-raw/skyline_meta-data.xlsx
@@ -1395,12 +1395,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D6" sqref="D6:E6"/>
+      <selection pane="topRight" activeCell="E8" sqref="E8:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,10 +1995,10 @@
         <v>250</v>
       </c>
       <c r="D8" s="3">
-        <v>44308</v>
+        <v>44316</v>
       </c>
       <c r="E8" s="3">
-        <v>44464</v>
+        <v>44361</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>172</v>
@@ -2007,7 +2006,7 @@
       <c r="G8" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>254</v>
       </c>
       <c r="I8" s="10">
@@ -2061,10 +2060,10 @@
         <v>250</v>
       </c>
       <c r="D9" s="3">
-        <v>44308</v>
+        <v>44316</v>
       </c>
       <c r="E9" s="3">
-        <v>44464</v>
+        <v>44361</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>172</v>
@@ -2126,10 +2125,10 @@
         <v>250</v>
       </c>
       <c r="D10" s="3">
-        <v>44308</v>
+        <v>44316</v>
       </c>
       <c r="E10" s="3">
-        <v>44464</v>
+        <v>44361</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>172</v>
@@ -2452,7 +2451,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>178</v>
       </c>
@@ -2510,13 +2509,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC15">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Picarro G2508"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor edits for split1; updated meta-data
</commit_message>
<xml_diff>
--- a/data-raw/skyline_meta-data.xlsx
+++ b/data-raw/skyline_meta-data.xlsx
@@ -1395,11 +1395,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E8" sqref="E8:E10"/>
+      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1414,7 @@
     <col min="9" max="9" width="15.7109375" style="11" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" style="11" customWidth="1"/>
     <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" customWidth="1"/>
+    <col min="12" max="12" width="111.7109375" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" style="11" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" style="11" customWidth="1"/>
     <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
@@ -1551,10 +1552,10 @@
         <v>256</v>
       </c>
       <c r="M2" s="10">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N2" s="10">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="O2" s="9" t="s">
         <v>225</v>
@@ -1562,14 +1563,14 @@
       <c r="P2" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="Q2" s="11">
-        <v>40</v>
+      <c r="Q2" s="10">
+        <v>24</v>
       </c>
       <c r="R2" s="10">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T2" t="s">
         <v>120</v>
@@ -1640,10 +1641,10 @@
         <v>264</v>
       </c>
       <c r="M3" s="10">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N3" s="10">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>225</v>
@@ -1651,14 +1652,14 @@
       <c r="P3" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="Q3" s="11">
-        <v>40</v>
+      <c r="Q3" s="10">
+        <v>24</v>
       </c>
       <c r="R3" s="10">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T3" t="s">
         <v>120</v>
@@ -1729,10 +1730,10 @@
         <v>264</v>
       </c>
       <c r="M4" s="10">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N4" s="10">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>225</v>
@@ -1740,14 +1741,14 @@
       <c r="P4" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="Q4" s="11">
-        <v>40</v>
+      <c r="Q4" s="10">
+        <v>24</v>
       </c>
       <c r="R4" s="10">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T4" t="s">
         <v>120</v>
@@ -1791,10 +1792,10 @@
         <v>247</v>
       </c>
       <c r="D5" s="3">
-        <v>43796</v>
+        <v>43854</v>
       </c>
       <c r="E5" s="3">
-        <v>44081</v>
+        <v>44054</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>172</v>
@@ -1818,10 +1819,10 @@
         <v>257</v>
       </c>
       <c r="M5" s="10">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N5" s="10">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>225</v>
@@ -1829,14 +1830,14 @@
       <c r="P5" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="Q5" s="11">
-        <v>40</v>
+      <c r="Q5" s="10">
+        <v>24</v>
       </c>
       <c r="R5" s="10">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T5" t="s">
         <v>120</v>
@@ -1859,10 +1860,10 @@
         <v>247</v>
       </c>
       <c r="D6" s="3">
-        <v>43796</v>
+        <v>43854</v>
       </c>
       <c r="E6" s="3">
-        <v>44081</v>
+        <v>44054</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>172</v>
@@ -1886,10 +1887,10 @@
         <v>265</v>
       </c>
       <c r="M6" s="10">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N6" s="10">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>225</v>
@@ -1897,14 +1898,14 @@
       <c r="P6" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="Q6" s="11">
-        <v>40</v>
+      <c r="Q6" s="10">
+        <v>24</v>
       </c>
       <c r="R6" s="10">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T6" t="s">
         <v>120</v>
@@ -1927,10 +1928,10 @@
         <v>247</v>
       </c>
       <c r="D7" s="3">
-        <v>43796</v>
+        <v>43854</v>
       </c>
       <c r="E7" s="3">
-        <v>44081</v>
+        <v>44054</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>172</v>
@@ -1954,10 +1955,10 @@
         <v>265</v>
       </c>
       <c r="M7" s="10">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N7" s="10">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="O7" s="9" t="s">
         <v>225</v>
@@ -1965,14 +1966,14 @@
       <c r="P7" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="Q7" s="11">
-        <v>40</v>
+      <c r="Q7" s="10">
+        <v>24</v>
       </c>
       <c r="R7" s="10">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T7" t="s">
         <v>120</v>
@@ -2179,7 +2180,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2383,7 +2384,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2451,7 +2452,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>178</v>
       </c>
@@ -2509,6 +2510,15 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AC15">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="biochar1"/>
+        <filter val="split1"/>
+        <filter val="yield1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
@@ -17022,6 +17032,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EF9ABF683E034F89344FAB5B39333E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dee778bbead9c5b03a2ef4f8fda037a0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b04e8096-b088-49dd-9bf5-7c33296d4394" xmlns:ns4="de44e333-4144-40ce-a2c0-3c7c2aff7df8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78a27167cd47c103910f2d57de5b9280" ns3:_="" ns4:_="">
     <xsd:import namespace="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
@@ -17250,36 +17275,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12485A3A-AC12-4EB2-89FF-E5633AE5EFB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33D70FC5-66D0-44F1-ACB8-BD99C781C922}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
-    <ds:schemaRef ds:uri="de44e333-4144-40ce-a2c0-3c7c2aff7df8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17302,9 +17301,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33D70FC5-66D0-44F1-ACB8-BD99C781C922}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12485A3A-AC12-4EB2-89FF-E5633AE5EFB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
+    <ds:schemaRef ds:uri="de44e333-4144-40ce-a2c0-3c7c2aff7df8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edits to work for Aeris - standardise names; read csv chpos data; filter mmnts where chpos sensor stuck, so n very large;
</commit_message>
<xml_diff>
--- a/data-raw/skyline_meta-data.xlsx
+++ b/data-raw/skyline_meta-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1950" windowWidth="29040" windowHeight="7260" tabRatio="836" activeTab="1"/>
+    <workbookView xWindow="-28920" yWindow="1950" windowWidth="29040" windowHeight="7260" tabRatio="836" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">chamber!$C$2:$C$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">experiment!$A$1:$AC$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">experiment!$A$1:$AC$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="273">
   <si>
     <t>DOC</t>
   </si>
@@ -730,9 +730,6 @@
     <t>local drive</t>
   </si>
   <si>
-    <t>JASMIN</t>
-  </si>
-  <si>
     <t>area_m2</t>
   </si>
   <si>
@@ -871,9 +868,6 @@
     <t>//nerclactdb.adceh.ceh.ac.uk/Projects/PROJECTS1/NEC05829 ASSIST/FIELD EXPT 3/Fluxes/RAW_DATA/Picarro_RAW</t>
   </si>
   <si>
-    <t>//nerclactdb.adceh.ceh.ac.uk/Projects/PROJECTS1/NEC07536 NERC DIVINE/WP2/Data/Fluxes/RAW_DATA/Aeris_RAW_old</t>
-  </si>
-  <si>
     <t>//nerclactdb.adceh.ceh.ac.uk/Projects/PROJECTS1/NEC05829 ASSIST/FIELD EXPT 1/Fluxes/RAW_DATA/CR1000_DAILY</t>
   </si>
   <si>
@@ -914,6 +908,21 @@
   </si>
   <si>
     <t>B1</t>
+  </si>
+  <si>
+    <t>data-raw/raw/HRG/diurnal1/chi_ghg</t>
+  </si>
+  <si>
+    <t>data-raw/raw/HRG/diurnal1/chamber_position</t>
+  </si>
+  <si>
+    <t>data-raw/raw/HRG/diurnal1/soil_met</t>
+  </si>
+  <si>
+    <t>%Y-%m-%d</t>
+  </si>
+  <si>
+    <t>//nerclactdb.adceh.ceh.ac.uk/Projects/PROJECTS1/NEC07536 NERC DIVINE/WP2/Data/Fluxes/RAW_DATA/Aeris_DAILY</t>
   </si>
 </sst>
 </file>
@@ -972,7 +981,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -992,6 +1001,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1396,11 +1408,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AC15"/>
+  <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M5" sqref="M5"/>
+      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,40 +1460,40 @@
         <v>205</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M1" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>173</v>
       </c>
       <c r="Q1" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="T1" t="s">
         <v>107</v>
@@ -1522,7 +1534,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D2" s="3">
         <v>43529</v>
@@ -1537,7 +1549,7 @@
         <v>206</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I2" s="10">
         <v>12</v>
@@ -1546,28 +1558,28 @@
         <v>26</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="M2" s="10">
         <v>24</v>
       </c>
       <c r="N2" s="10">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="O2" s="9" t="s">
         <v>225</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="Q2" s="10">
         <v>24</v>
       </c>
       <c r="R2" s="10">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>225</v>
@@ -1611,7 +1623,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D3" s="3">
         <v>43529</v>
@@ -1626,7 +1638,7 @@
         <v>207</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I3" s="10">
         <v>12</v>
@@ -1635,28 +1647,28 @@
         <v>26</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M3" s="10">
         <v>24</v>
       </c>
       <c r="N3" s="10">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>225</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="Q3" s="10">
         <v>24</v>
       </c>
       <c r="R3" s="10">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="S3" s="9" t="s">
         <v>225</v>
@@ -1696,26 +1708,26 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
+      <c r="B4" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D4" s="3">
-        <v>43529</v>
+        <v>43854</v>
       </c>
       <c r="E4" s="3">
-        <v>43733</v>
+        <v>44054</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>172</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>261</v>
+        <v>206</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="I4" s="10">
         <v>12</v>
@@ -1724,10 +1736,10 @@
         <v>26</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>264</v>
+        <v>217</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>255</v>
       </c>
       <c r="M4" s="10">
         <v>24</v>
@@ -1736,10 +1748,10 @@
         <v>38</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>266</v>
+        <v>224</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>255</v>
       </c>
       <c r="Q4" s="10">
         <v>24</v>
@@ -1748,37 +1760,16 @@
         <v>38</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T4" t="s">
         <v>120</v>
       </c>
-      <c r="U4" t="s">
-        <v>121</v>
+      <c r="U4" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="V4" t="s">
-        <v>122</v>
-      </c>
-      <c r="W4" t="s">
-        <v>111</v>
-      </c>
-      <c r="X4" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
@@ -1786,10 +1777,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D5" s="3">
         <v>43854</v>
@@ -1801,10 +1792,10 @@
         <v>172</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>253</v>
+        <v>207</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>260</v>
       </c>
       <c r="I5" s="10">
         <v>12</v>
@@ -1813,10 +1804,10 @@
         <v>26</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>257</v>
+        <v>217</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>263</v>
       </c>
       <c r="M5" s="10">
         <v>24</v>
@@ -1825,10 +1816,10 @@
         <v>38</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>257</v>
+        <v>224</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>265</v>
       </c>
       <c r="Q5" s="10">
         <v>24</v>
@@ -1837,7 +1828,7 @@
         <v>38</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T5" t="s">
         <v>120</v>
@@ -1849,30 +1840,30 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>245</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D6" s="3">
-        <v>43854</v>
+        <v>44316</v>
       </c>
       <c r="E6" s="3">
-        <v>44054</v>
+        <v>44361</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>172</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>262</v>
+        <v>206</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="I6" s="10">
         <v>12</v>
@@ -1881,28 +1872,28 @@
         <v>26</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>265</v>
+        <v>217</v>
+      </c>
+      <c r="L6" t="s">
+        <v>256</v>
       </c>
       <c r="M6" s="10">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="N6" s="10">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>267</v>
+        <v>224</v>
+      </c>
+      <c r="P6" t="s">
+        <v>256</v>
       </c>
       <c r="Q6" s="10">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="R6" s="10">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="S6" s="9" t="s">
         <v>225</v>
@@ -1910,37 +1901,34 @@
       <c r="T6" t="s">
         <v>120</v>
       </c>
-      <c r="U6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="V6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U6" s="12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>245</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D7" s="3">
-        <v>43854</v>
+        <v>44316</v>
       </c>
       <c r="E7" s="3">
-        <v>44054</v>
+        <v>44361</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>172</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I7" s="10">
         <v>12</v>
@@ -1949,28 +1937,28 @@
         <v>26</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M7" s="10">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="N7" s="10">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q7" s="10">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="R7" s="10">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="S7" s="9" t="s">
         <v>225</v>
@@ -1978,28 +1966,25 @@
       <c r="T7" t="s">
         <v>120</v>
       </c>
-      <c r="U7" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="V7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U7" s="12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>246</v>
+      <c r="B8" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D8" s="3">
-        <v>44316</v>
+        <v>45001</v>
       </c>
       <c r="E8" s="3">
-        <v>44361</v>
+        <v>45150</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>172</v>
@@ -2007,8 +1992,8 @@
       <c r="G8" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>254</v>
+      <c r="H8" s="9" t="s">
+        <v>202</v>
       </c>
       <c r="I8" s="10">
         <v>12</v>
@@ -2017,63 +2002,66 @@
         <v>26</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="L8" t="s">
-        <v>258</v>
+        <v>217</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>204</v>
       </c>
       <c r="M8" s="10">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="N8" s="10">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="O8" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>40</v>
+      </c>
+      <c r="R8" s="10">
+        <v>49</v>
+      </c>
+      <c r="S8" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="P8" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>32</v>
-      </c>
-      <c r="R8" s="10">
-        <v>46</v>
-      </c>
-      <c r="S8" s="9" t="s">
-        <v>226</v>
-      </c>
       <c r="T8" t="s">
         <v>120</v>
       </c>
-      <c r="U8" s="12" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U8" t="s">
+        <v>150</v>
+      </c>
+      <c r="V8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>246</v>
+        <v>164</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D9" s="3">
-        <v>44316</v>
+        <v>45001</v>
       </c>
       <c r="E9" s="3">
-        <v>44361</v>
+        <v>45150</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>172</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>263</v>
+        <v>202</v>
       </c>
       <c r="I9" s="10">
         <v>12</v>
@@ -2082,63 +2070,66 @@
         <v>26</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>268</v>
+        <v>204</v>
       </c>
       <c r="M9" s="10">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="N9" s="10">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="O9" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>40</v>
+      </c>
+      <c r="R9" s="10">
+        <v>49</v>
+      </c>
+      <c r="S9" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="P9" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>32</v>
-      </c>
-      <c r="R9" s="10">
-        <v>46</v>
-      </c>
-      <c r="S9" s="9" t="s">
-        <v>226</v>
-      </c>
       <c r="T9" t="s">
         <v>120</v>
       </c>
-      <c r="U9" s="12" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="U9" t="s">
+        <v>150</v>
+      </c>
+      <c r="V9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D10" s="3">
-        <v>44316</v>
+        <v>45001</v>
       </c>
       <c r="E10" s="3">
-        <v>44361</v>
+        <v>45150</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>172</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>263</v>
+        <v>211</v>
       </c>
       <c r="I10" s="10">
         <v>12</v>
@@ -2147,373 +2138,188 @@
         <v>26</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>268</v>
+        <v>209</v>
       </c>
       <c r="M10" s="10">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="N10" s="10">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="O10" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>40</v>
+      </c>
+      <c r="R10" s="10">
+        <v>49</v>
+      </c>
+      <c r="S10" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="P10" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q10" s="10">
-        <v>32</v>
-      </c>
-      <c r="R10" s="10">
-        <v>46</v>
-      </c>
-      <c r="S10" s="9" t="s">
-        <v>226</v>
-      </c>
       <c r="T10" t="s">
         <v>120</v>
       </c>
-      <c r="U10" s="12" t="s">
-        <v>269</v>
+      <c r="U10" t="s">
+        <v>150</v>
+      </c>
+      <c r="V10" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>251</v>
+        <v>178</v>
+      </c>
+      <c r="B11" t="s">
+        <v>146</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D11" s="3">
-        <v>45001</v>
-      </c>
-      <c r="E11" s="3">
-        <v>45150</v>
+        <v>147</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E11" s="8">
+        <v>45184.520833333336</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>202</v>
+      <c r="H11" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="I11" s="10">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J11" s="10">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>204</v>
+        <v>271</v>
+      </c>
+      <c r="L11" t="s">
+        <v>257</v>
       </c>
       <c r="M11" s="10">
-        <v>21</v>
-      </c>
-      <c r="N11" s="10">
-        <v>35</v>
+        <v>29</v>
+      </c>
+      <c r="N11" s="13">
+        <v>38</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="P11" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q11" s="11">
-        <v>40</v>
-      </c>
-      <c r="R11" s="10">
-        <v>49</v>
+        <v>271</v>
+      </c>
+      <c r="P11" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>25</v>
+      </c>
+      <c r="R11" s="13">
+        <v>34</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>226</v>
+        <v>271</v>
       </c>
       <c r="T11" t="s">
         <v>120</v>
       </c>
       <c r="U11" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
       <c r="V11" t="s">
-        <v>151</v>
+        <v>182</v>
+      </c>
+      <c r="W11" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D12" s="3">
-        <v>45001</v>
-      </c>
-      <c r="E12" s="3">
-        <v>45150</v>
+        <v>147</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="8">
+        <v>45184.520833333336</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>202</v>
+        <v>268</v>
       </c>
       <c r="I12" s="10">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="J12" s="10">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>218</v>
+        <v>271</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>204</v>
+        <v>269</v>
       </c>
       <c r="M12" s="10">
-        <v>21</v>
-      </c>
-      <c r="N12" s="10">
-        <v>35</v>
+        <v>29</v>
+      </c>
+      <c r="N12" s="13">
+        <v>38</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>225</v>
+        <v>271</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q12" s="11">
-        <v>40</v>
-      </c>
-      <c r="R12" s="10">
-        <v>49</v>
+        <v>270</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>25</v>
+      </c>
+      <c r="R12" s="13">
+        <v>34</v>
       </c>
       <c r="S12" s="9" t="s">
-        <v>226</v>
+        <v>271</v>
       </c>
       <c r="T12" t="s">
         <v>120</v>
       </c>
       <c r="U12" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
       <c r="V12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D13" s="3">
-        <v>45001</v>
-      </c>
-      <c r="E13" s="3">
-        <v>45150</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="I13" s="10">
-        <v>12</v>
-      </c>
-      <c r="J13" s="10">
-        <v>26</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="M13" s="10">
-        <v>21</v>
-      </c>
-      <c r="N13" s="10">
-        <v>35</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="P13" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q13" s="11">
-        <v>40</v>
-      </c>
-      <c r="R13" s="10">
-        <v>49</v>
-      </c>
-      <c r="S13" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="T13" t="s">
-        <v>120</v>
-      </c>
-      <c r="U13" t="s">
-        <v>150</v>
-      </c>
-      <c r="V13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D14" s="3">
-        <v>45001</v>
-      </c>
-      <c r="E14" s="3">
-        <v>45150</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="I14" s="10">
-        <v>12</v>
-      </c>
-      <c r="J14" s="10">
-        <v>26</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="M14" s="10">
-        <v>21</v>
-      </c>
-      <c r="N14" s="10">
-        <v>35</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="P14" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q14" s="11">
-        <v>40</v>
-      </c>
-      <c r="R14" s="10">
-        <v>49</v>
-      </c>
-      <c r="S14" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="T14" t="s">
-        <v>120</v>
-      </c>
-      <c r="U14" t="s">
-        <v>150</v>
-      </c>
-      <c r="V14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>178</v>
-      </c>
-      <c r="B15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="8">
-        <v>45184.520833333336</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="H15" t="s">
-        <v>255</v>
-      </c>
-      <c r="I15" s="10">
-        <v>12</v>
-      </c>
-      <c r="J15" s="10">
-        <v>26</v>
-      </c>
-      <c r="L15" t="s">
-        <v>259</v>
-      </c>
-      <c r="M15" s="10">
-        <v>21</v>
-      </c>
-      <c r="P15" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q15" s="11">
-        <v>40</v>
-      </c>
-      <c r="S15" s="9"/>
-      <c r="T15" t="s">
-        <v>120</v>
-      </c>
-      <c r="U15" t="s">
-        <v>181</v>
-      </c>
-      <c r="V15" t="s">
         <v>182</v>
       </c>
-      <c r="W15" t="s">
+      <c r="W12" t="s">
         <v>183</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC15">
+  <autoFilter ref="A1:AC12">
     <filterColumn colId="1">
       <filters>
-        <filter val="biochar1"/>
         <filter val="split1"/>
         <filter val="yield1"/>
       </filters>
@@ -5493,7 +5299,7 @@
   <dimension ref="A1:J374"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A347" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D374" sqref="D374"/>
     </sheetView>
   </sheetViews>
@@ -5521,7 +5327,7 @@
         <v>131</v>
       </c>
       <c r="E1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F1" t="s">
         <v>174</v>
@@ -13760,7 +13566,7 @@
         <v>9</v>
       </c>
       <c r="B318" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C318" t="s">
         <v>120</v>
@@ -13786,7 +13592,7 @@
         <v>9</v>
       </c>
       <c r="B319" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C319" t="s">
         <v>120</v>
@@ -13812,7 +13618,7 @@
         <v>9</v>
       </c>
       <c r="B320" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C320" t="s">
         <v>120</v>
@@ -13838,7 +13644,7 @@
         <v>9</v>
       </c>
       <c r="B321" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C321" t="s">
         <v>120</v>
@@ -13864,7 +13670,7 @@
         <v>9</v>
       </c>
       <c r="B322" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C322" t="s">
         <v>120</v>
@@ -13890,7 +13696,7 @@
         <v>9</v>
       </c>
       <c r="B323" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C323" t="s">
         <v>120</v>
@@ -13916,7 +13722,7 @@
         <v>9</v>
       </c>
       <c r="B324" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C324" t="s">
         <v>120</v>
@@ -13942,7 +13748,7 @@
         <v>9</v>
       </c>
       <c r="B325" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C325" t="s">
         <v>120</v>
@@ -13968,7 +13774,7 @@
         <v>9</v>
       </c>
       <c r="B326" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C326" t="s">
         <v>120</v>
@@ -13994,7 +13800,7 @@
         <v>9</v>
       </c>
       <c r="B327" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C327" t="s">
         <v>120</v>
@@ -14020,7 +13826,7 @@
         <v>9</v>
       </c>
       <c r="B328" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C328" t="s">
         <v>120</v>
@@ -14046,7 +13852,7 @@
         <v>9</v>
       </c>
       <c r="B329" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C329" t="s">
         <v>120</v>
@@ -14072,7 +13878,7 @@
         <v>9</v>
       </c>
       <c r="B330" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C330" t="s">
         <v>120</v>
@@ -14098,7 +13904,7 @@
         <v>9</v>
       </c>
       <c r="B331" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C331" t="s">
         <v>120</v>
@@ -14124,7 +13930,7 @@
         <v>9</v>
       </c>
       <c r="B332" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C332" t="s">
         <v>120</v>
@@ -14150,7 +13956,7 @@
         <v>9</v>
       </c>
       <c r="B333" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C333" t="s">
         <v>120</v>
@@ -14176,7 +13982,7 @@
         <v>9</v>
       </c>
       <c r="B334" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C334" t="s">
         <v>120</v>
@@ -14202,7 +14008,7 @@
         <v>9</v>
       </c>
       <c r="B335" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C335" t="s">
         <v>120</v>
@@ -14228,7 +14034,7 @@
         <v>9</v>
       </c>
       <c r="B336" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C336" t="s">
         <v>120</v>
@@ -14254,7 +14060,7 @@
         <v>9</v>
       </c>
       <c r="B337" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C337" t="s">
         <v>120</v>
@@ -14280,7 +14086,7 @@
         <v>9</v>
       </c>
       <c r="B338" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C338" t="s">
         <v>120</v>
@@ -14306,7 +14112,7 @@
         <v>9</v>
       </c>
       <c r="B339" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C339" t="s">
         <v>120</v>
@@ -14332,7 +14138,7 @@
         <v>9</v>
       </c>
       <c r="B340" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C340" t="s">
         <v>120</v>
@@ -14358,7 +14164,7 @@
         <v>9</v>
       </c>
       <c r="B341" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C341" t="s">
         <v>120</v>
@@ -14384,7 +14190,7 @@
         <v>9</v>
       </c>
       <c r="B342" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C342" t="s">
         <v>120</v>
@@ -14410,7 +14216,7 @@
         <v>9</v>
       </c>
       <c r="B343" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C343" t="s">
         <v>120</v>
@@ -14436,7 +14242,7 @@
         <v>9</v>
       </c>
       <c r="B344" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C344" t="s">
         <v>120</v>
@@ -14462,7 +14268,7 @@
         <v>9</v>
       </c>
       <c r="B345" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C345" t="s">
         <v>120</v>
@@ -14488,7 +14294,7 @@
         <v>9</v>
       </c>
       <c r="B346" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C346" t="s">
         <v>120</v>
@@ -14514,7 +14320,7 @@
         <v>9</v>
       </c>
       <c r="B347" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C347" t="s">
         <v>120</v>
@@ -14540,7 +14346,7 @@
         <v>9</v>
       </c>
       <c r="B348" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C348" t="s">
         <v>120</v>
@@ -14566,7 +14372,7 @@
         <v>9</v>
       </c>
       <c r="B349" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C349" t="s">
         <v>120</v>
@@ -14592,7 +14398,7 @@
         <v>9</v>
       </c>
       <c r="B350" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C350" t="s">
         <v>120</v>
@@ -14618,7 +14424,7 @@
         <v>9</v>
       </c>
       <c r="B351" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C351" t="s">
         <v>120</v>
@@ -14644,7 +14450,7 @@
         <v>9</v>
       </c>
       <c r="B352" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C352" t="s">
         <v>120</v>
@@ -14670,7 +14476,7 @@
         <v>9</v>
       </c>
       <c r="B353" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C353" t="s">
         <v>120</v>
@@ -14696,7 +14502,7 @@
         <v>9</v>
       </c>
       <c r="B354" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C354" t="s">
         <v>120</v>
@@ -14722,7 +14528,7 @@
         <v>9</v>
       </c>
       <c r="B355" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C355" t="s">
         <v>120</v>
@@ -15541,7 +15347,7 @@
         <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E2" s="2">
         <v>36526.4375</v>
@@ -15576,7 +15382,7 @@
         <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E3" s="2">
         <v>36526.4375</v>
@@ -15611,7 +15417,7 @@
         <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E4" s="2">
         <v>36526.4375</v>
@@ -15646,7 +15452,7 @@
         <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E5" s="2">
         <v>36526.4375</v>
@@ -15681,7 +15487,7 @@
         <v>120</v>
       </c>
       <c r="D6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E6" s="2">
         <v>36526.4375</v>
@@ -15716,7 +15522,7 @@
         <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E7" s="2">
         <v>36526.4375</v>
@@ -15751,7 +15557,7 @@
         <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E8" s="2">
         <v>36526.4375</v>
@@ -15786,7 +15592,7 @@
         <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E9" s="2">
         <v>36526.4375</v>
@@ -15821,7 +15627,7 @@
         <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E10" s="2">
         <v>36557.4375</v>
@@ -15856,7 +15662,7 @@
         <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E11" s="2">
         <v>36557.4375</v>
@@ -15891,7 +15697,7 @@
         <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E12" s="2">
         <v>36557.4375</v>
@@ -15926,7 +15732,7 @@
         <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E13" s="2">
         <v>36557.4375</v>
@@ -15961,7 +15767,7 @@
         <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E14" s="2">
         <v>36557.4375</v>
@@ -15996,7 +15802,7 @@
         <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E15" s="2">
         <v>36557.4375</v>
@@ -16031,7 +15837,7 @@
         <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E16" s="2">
         <v>36557.4375</v>
@@ -16066,7 +15872,7 @@
         <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E17" s="2">
         <v>36557.4375</v>
@@ -16101,7 +15907,7 @@
         <v>151</v>
       </c>
       <c r="D18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E18" s="3">
         <v>44965</v>
@@ -16130,7 +15936,7 @@
         <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E19" s="3">
         <v>44965</v>
@@ -16160,7 +15966,7 @@
         <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E20" s="3">
         <v>44965</v>
@@ -16190,7 +15996,7 @@
         <v>150</v>
       </c>
       <c r="D21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E21" s="3">
         <v>44965</v>
@@ -16220,7 +16026,7 @@
         <v>150</v>
       </c>
       <c r="D22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E22" s="3">
         <v>44965</v>
@@ -16250,7 +16056,7 @@
         <v>120</v>
       </c>
       <c r="D23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E23" s="3">
         <v>44965</v>
@@ -16280,7 +16086,7 @@
         <v>150</v>
       </c>
       <c r="D24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E24" s="3">
         <v>44965</v>
@@ -16310,7 +16116,7 @@
         <v>151</v>
       </c>
       <c r="D25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E25" s="3">
         <v>44965</v>
@@ -16340,7 +16146,7 @@
         <v>150</v>
       </c>
       <c r="D26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E26" s="3">
         <v>44965</v>
@@ -16370,7 +16176,7 @@
         <v>151</v>
       </c>
       <c r="D27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E27" s="3">
         <v>44965</v>
@@ -16400,7 +16206,7 @@
         <v>151</v>
       </c>
       <c r="D28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E28" s="3">
         <v>44965</v>
@@ -16430,7 +16236,7 @@
         <v>120</v>
       </c>
       <c r="D29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E29" s="3">
         <v>44965</v>
@@ -16460,7 +16266,7 @@
         <v>151</v>
       </c>
       <c r="D30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E30" s="3">
         <v>44965</v>
@@ -16490,7 +16296,7 @@
         <v>120</v>
       </c>
       <c r="D31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E31" s="3">
         <v>44965</v>
@@ -16520,7 +16326,7 @@
         <v>120</v>
       </c>
       <c r="D32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E32" s="3">
         <v>44965</v>
@@ -16550,7 +16356,7 @@
         <v>151</v>
       </c>
       <c r="D33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E33" s="3">
         <v>44965</v>
@@ -16580,7 +16386,7 @@
         <v>150</v>
       </c>
       <c r="D34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E34" s="3">
         <v>44965</v>
@@ -16610,7 +16416,7 @@
         <v>150</v>
       </c>
       <c r="D35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E35" s="3">
         <v>44965</v>
@@ -17032,21 +16838,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EF9ABF683E034F89344FAB5B39333E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dee778bbead9c5b03a2ef4f8fda037a0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b04e8096-b088-49dd-9bf5-7c33296d4394" xmlns:ns4="de44e333-4144-40ce-a2c0-3c7c2aff7df8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78a27167cd47c103910f2d57de5b9280" ns3:_="" ns4:_="">
     <xsd:import namespace="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
@@ -17275,32 +17066,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33D70FC5-66D0-44F1-ACB8-BD99C781C922}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1591EC7B-C469-4BBA-B7FD-C66217A363C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de44e333-4144-40ce-a2c0-3c7c2aff7df8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12485A3A-AC12-4EB2-89FF-E5633AE5EFB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17317,4 +17098,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1591EC7B-C469-4BBA-B7FD-C66217A363C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="de44e333-4144-40ce-a2c0-3c7c2aff7df8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33D70FC5-66D0-44F1-ACB8-BD99C781C922}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reshape soilmet data and join; correct treatment meta-data (C_55)
</commit_message>
<xml_diff>
--- a/data-raw/skyline_meta-data.xlsx
+++ b/data-raw/skyline_meta-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1950" windowWidth="29040" windowHeight="7260" tabRatio="836" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-28920" yWindow="1950" windowWidth="29040" windowHeight="4125" tabRatio="836" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="2" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="272">
   <si>
     <t>DOC</t>
   </si>
@@ -704,9 +704,6 @@
   </si>
   <si>
     <t>04/05/2023  14:50:00</t>
-  </si>
-  <si>
-    <t>C_55</t>
   </si>
   <si>
     <t>trmt_name</t>
@@ -1410,9 +1407,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P2" sqref="P2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,43 +1454,43 @@
         <v>171</v>
       </c>
       <c r="G1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M1" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>173</v>
       </c>
       <c r="Q1" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="T1" t="s">
         <v>107</v>
@@ -1526,7 +1523,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1534,7 +1531,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D2" s="3">
         <v>43529</v>
@@ -1546,10 +1543,10 @@
         <v>172</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I2" s="10">
         <v>12</v>
@@ -1558,10 +1555,10 @@
         <v>26</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M2" s="10">
         <v>24</v>
@@ -1570,10 +1567,10 @@
         <v>33</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q2" s="10">
         <v>24</v>
@@ -1582,7 +1579,7 @@
         <v>33</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T2" t="s">
         <v>120</v>
@@ -1615,7 +1612,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1623,7 +1620,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D3" s="3">
         <v>43529</v>
@@ -1635,10 +1632,10 @@
         <v>172</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I3" s="10">
         <v>12</v>
@@ -1647,10 +1644,10 @@
         <v>26</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M3" s="10">
         <v>24</v>
@@ -1659,10 +1656,10 @@
         <v>33</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q3" s="10">
         <v>24</v>
@@ -1671,7 +1668,7 @@
         <v>33</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T3" t="s">
         <v>120</v>
@@ -1704,15 +1701,15 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D4" s="3">
         <v>43854</v>
@@ -1724,10 +1721,10 @@
         <v>172</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I4" s="10">
         <v>12</v>
@@ -1736,10 +1733,10 @@
         <v>26</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M4" s="10">
         <v>24</v>
@@ -1748,10 +1745,10 @@
         <v>38</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q4" s="10">
         <v>24</v>
@@ -1760,7 +1757,7 @@
         <v>38</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="T4" t="s">
         <v>120</v>
@@ -1772,15 +1769,15 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D5" s="3">
         <v>43854</v>
@@ -1792,10 +1789,10 @@
         <v>172</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I5" s="10">
         <v>12</v>
@@ -1804,10 +1801,10 @@
         <v>26</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M5" s="10">
         <v>24</v>
@@ -1816,10 +1813,10 @@
         <v>38</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q5" s="10">
         <v>24</v>
@@ -1828,7 +1825,7 @@
         <v>38</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="T5" t="s">
         <v>120</v>
@@ -1845,10 +1842,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D6" s="3">
         <v>44316</v>
@@ -1860,10 +1857,10 @@
         <v>172</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I6" s="10">
         <v>12</v>
@@ -1872,10 +1869,10 @@
         <v>26</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M6" s="10">
         <v>32</v>
@@ -1884,10 +1881,10 @@
         <v>46</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q6" s="10">
         <v>32</v>
@@ -1896,13 +1893,13 @@
         <v>46</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T6" t="s">
         <v>120</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
@@ -1910,10 +1907,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D7" s="3">
         <v>44316</v>
@@ -1925,10 +1922,10 @@
         <v>172</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I7" s="10">
         <v>12</v>
@@ -1937,10 +1934,10 @@
         <v>26</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M7" s="10">
         <v>32</v>
@@ -1949,10 +1946,10 @@
         <v>46</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Q7" s="10">
         <v>32</v>
@@ -1961,13 +1958,13 @@
         <v>46</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T7" t="s">
         <v>120</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
@@ -1975,10 +1972,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D8" s="3">
         <v>45001</v>
@@ -1990,10 +1987,10 @@
         <v>172</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I8" s="10">
         <v>12</v>
@@ -2002,10 +1999,10 @@
         <v>26</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M8" s="10">
         <v>21</v>
@@ -2014,10 +2011,10 @@
         <v>35</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q8" s="11">
         <v>40</v>
@@ -2026,7 +2023,7 @@
         <v>49</v>
       </c>
       <c r="S8" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T8" t="s">
         <v>120</v>
@@ -2046,7 +2043,7 @@
         <v>164</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D9" s="3">
         <v>45001</v>
@@ -2058,10 +2055,10 @@
         <v>172</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I9" s="10">
         <v>12</v>
@@ -2070,10 +2067,10 @@
         <v>26</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M9" s="10">
         <v>21</v>
@@ -2082,10 +2079,10 @@
         <v>35</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q9" s="11">
         <v>40</v>
@@ -2094,7 +2091,7 @@
         <v>49</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T9" t="s">
         <v>120</v>
@@ -2114,7 +2111,7 @@
         <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D10" s="3">
         <v>45001</v>
@@ -2126,10 +2123,10 @@
         <v>172</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I10" s="10">
         <v>12</v>
@@ -2138,10 +2135,10 @@
         <v>26</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M10" s="10">
         <v>21</v>
@@ -2150,10 +2147,10 @@
         <v>35</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q10" s="11">
         <v>40</v>
@@ -2162,7 +2159,7 @@
         <v>49</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T10" t="s">
         <v>120</v>
@@ -2174,7 +2171,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>178</v>
       </c>
@@ -2194,10 +2191,10 @@
         <v>180</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I11" s="10">
         <v>1</v>
@@ -2206,10 +2203,10 @@
         <v>10</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M11" s="10">
         <v>29</v>
@@ -2218,10 +2215,10 @@
         <v>38</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="P11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q11" s="10">
         <v>25</v>
@@ -2230,7 +2227,7 @@
         <v>34</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="T11" t="s">
         <v>120</v>
@@ -2245,7 +2242,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>178</v>
       </c>
@@ -2265,10 +2262,10 @@
         <v>180</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I12" s="10">
         <v>1</v>
@@ -2277,10 +2274,10 @@
         <v>10</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M12" s="10">
         <v>29</v>
@@ -2289,10 +2286,10 @@
         <v>38</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q12" s="10">
         <v>25</v>
@@ -2301,7 +2298,7 @@
         <v>34</v>
       </c>
       <c r="S12" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="T12" t="s">
         <v>120</v>
@@ -2320,8 +2317,7 @@
   <autoFilter ref="A1:AC12">
     <filterColumn colId="1">
       <filters>
-        <filter val="split1"/>
-        <filter val="yield1"/>
+        <filter val="diurnal1"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2334,8 +2330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,7 +2351,7 @@
         <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5299,8 +5295,8 @@
   <dimension ref="A1:J374"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D374" sqref="D374"/>
+      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C287" sqref="C287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5327,7 +5323,7 @@
         <v>131</v>
       </c>
       <c r="E1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F1" t="s">
         <v>174</v>
@@ -8083,7 +8079,7 @@
         <v>146</v>
       </c>
       <c r="C107" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="D107">
         <v>10</v>
@@ -12763,7 +12759,7 @@
         <v>146</v>
       </c>
       <c r="C287" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="D287">
         <v>10</v>
@@ -13566,7 +13562,7 @@
         <v>9</v>
       </c>
       <c r="B318" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C318" t="s">
         <v>120</v>
@@ -13592,7 +13588,7 @@
         <v>9</v>
       </c>
       <c r="B319" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C319" t="s">
         <v>120</v>
@@ -13618,7 +13614,7 @@
         <v>9</v>
       </c>
       <c r="B320" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C320" t="s">
         <v>120</v>
@@ -13644,7 +13640,7 @@
         <v>9</v>
       </c>
       <c r="B321" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C321" t="s">
         <v>120</v>
@@ -13670,7 +13666,7 @@
         <v>9</v>
       </c>
       <c r="B322" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C322" t="s">
         <v>120</v>
@@ -13696,7 +13692,7 @@
         <v>9</v>
       </c>
       <c r="B323" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C323" t="s">
         <v>120</v>
@@ -13722,7 +13718,7 @@
         <v>9</v>
       </c>
       <c r="B324" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C324" t="s">
         <v>120</v>
@@ -13748,7 +13744,7 @@
         <v>9</v>
       </c>
       <c r="B325" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C325" t="s">
         <v>120</v>
@@ -13774,7 +13770,7 @@
         <v>9</v>
       </c>
       <c r="B326" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C326" t="s">
         <v>120</v>
@@ -13800,7 +13796,7 @@
         <v>9</v>
       </c>
       <c r="B327" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C327" t="s">
         <v>120</v>
@@ -13826,7 +13822,7 @@
         <v>9</v>
       </c>
       <c r="B328" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C328" t="s">
         <v>120</v>
@@ -13852,7 +13848,7 @@
         <v>9</v>
       </c>
       <c r="B329" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C329" t="s">
         <v>120</v>
@@ -13878,7 +13874,7 @@
         <v>9</v>
       </c>
       <c r="B330" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C330" t="s">
         <v>120</v>
@@ -13904,7 +13900,7 @@
         <v>9</v>
       </c>
       <c r="B331" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C331" t="s">
         <v>120</v>
@@ -13930,7 +13926,7 @@
         <v>9</v>
       </c>
       <c r="B332" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C332" t="s">
         <v>120</v>
@@ -13956,7 +13952,7 @@
         <v>9</v>
       </c>
       <c r="B333" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C333" t="s">
         <v>120</v>
@@ -13982,7 +13978,7 @@
         <v>9</v>
       </c>
       <c r="B334" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C334" t="s">
         <v>120</v>
@@ -14008,7 +14004,7 @@
         <v>9</v>
       </c>
       <c r="B335" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C335" t="s">
         <v>120</v>
@@ -14034,7 +14030,7 @@
         <v>9</v>
       </c>
       <c r="B336" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C336" t="s">
         <v>120</v>
@@ -14060,7 +14056,7 @@
         <v>9</v>
       </c>
       <c r="B337" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C337" t="s">
         <v>120</v>
@@ -14086,7 +14082,7 @@
         <v>9</v>
       </c>
       <c r="B338" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C338" t="s">
         <v>120</v>
@@ -14112,7 +14108,7 @@
         <v>9</v>
       </c>
       <c r="B339" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C339" t="s">
         <v>120</v>
@@ -14138,7 +14134,7 @@
         <v>9</v>
       </c>
       <c r="B340" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C340" t="s">
         <v>120</v>
@@ -14164,7 +14160,7 @@
         <v>9</v>
       </c>
       <c r="B341" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C341" t="s">
         <v>120</v>
@@ -14190,7 +14186,7 @@
         <v>9</v>
       </c>
       <c r="B342" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C342" t="s">
         <v>120</v>
@@ -14216,7 +14212,7 @@
         <v>9</v>
       </c>
       <c r="B343" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C343" t="s">
         <v>120</v>
@@ -14242,7 +14238,7 @@
         <v>9</v>
       </c>
       <c r="B344" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C344" t="s">
         <v>120</v>
@@ -14268,7 +14264,7 @@
         <v>9</v>
       </c>
       <c r="B345" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C345" t="s">
         <v>120</v>
@@ -14294,7 +14290,7 @@
         <v>9</v>
       </c>
       <c r="B346" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C346" t="s">
         <v>120</v>
@@ -14320,7 +14316,7 @@
         <v>9</v>
       </c>
       <c r="B347" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C347" t="s">
         <v>120</v>
@@ -14346,7 +14342,7 @@
         <v>9</v>
       </c>
       <c r="B348" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C348" t="s">
         <v>120</v>
@@ -14372,7 +14368,7 @@
         <v>9</v>
       </c>
       <c r="B349" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C349" t="s">
         <v>120</v>
@@ -14398,7 +14394,7 @@
         <v>9</v>
       </c>
       <c r="B350" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C350" t="s">
         <v>120</v>
@@ -14424,7 +14420,7 @@
         <v>9</v>
       </c>
       <c r="B351" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C351" t="s">
         <v>120</v>
@@ -14450,7 +14446,7 @@
         <v>9</v>
       </c>
       <c r="B352" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C352" t="s">
         <v>120</v>
@@ -14476,7 +14472,7 @@
         <v>9</v>
       </c>
       <c r="B353" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C353" t="s">
         <v>120</v>
@@ -14502,7 +14498,7 @@
         <v>9</v>
       </c>
       <c r="B354" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C354" t="s">
         <v>120</v>
@@ -14528,7 +14524,7 @@
         <v>9</v>
       </c>
       <c r="B355" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C355" t="s">
         <v>120</v>
@@ -15347,7 +15343,7 @@
         <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E2" s="2">
         <v>36526.4375</v>
@@ -15382,7 +15378,7 @@
         <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E3" s="2">
         <v>36526.4375</v>
@@ -15417,7 +15413,7 @@
         <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E4" s="2">
         <v>36526.4375</v>
@@ -15452,7 +15448,7 @@
         <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E5" s="2">
         <v>36526.4375</v>
@@ -15487,7 +15483,7 @@
         <v>120</v>
       </c>
       <c r="D6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E6" s="2">
         <v>36526.4375</v>
@@ -15522,7 +15518,7 @@
         <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E7" s="2">
         <v>36526.4375</v>
@@ -15557,7 +15553,7 @@
         <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E8" s="2">
         <v>36526.4375</v>
@@ -15592,7 +15588,7 @@
         <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E9" s="2">
         <v>36526.4375</v>
@@ -15627,7 +15623,7 @@
         <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E10" s="2">
         <v>36557.4375</v>
@@ -15662,7 +15658,7 @@
         <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E11" s="2">
         <v>36557.4375</v>
@@ -15697,7 +15693,7 @@
         <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E12" s="2">
         <v>36557.4375</v>
@@ -15732,7 +15728,7 @@
         <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E13" s="2">
         <v>36557.4375</v>
@@ -15767,7 +15763,7 @@
         <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E14" s="2">
         <v>36557.4375</v>
@@ -15802,7 +15798,7 @@
         <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E15" s="2">
         <v>36557.4375</v>
@@ -15837,7 +15833,7 @@
         <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E16" s="2">
         <v>36557.4375</v>
@@ -15872,7 +15868,7 @@
         <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E17" s="2">
         <v>36557.4375</v>
@@ -15907,7 +15903,7 @@
         <v>151</v>
       </c>
       <c r="D18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E18" s="3">
         <v>44965</v>
@@ -15936,7 +15932,7 @@
         <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E19" s="3">
         <v>44965</v>
@@ -15966,7 +15962,7 @@
         <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E20" s="3">
         <v>44965</v>
@@ -15996,7 +15992,7 @@
         <v>150</v>
       </c>
       <c r="D21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E21" s="3">
         <v>44965</v>
@@ -16026,7 +16022,7 @@
         <v>150</v>
       </c>
       <c r="D22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E22" s="3">
         <v>44965</v>
@@ -16056,7 +16052,7 @@
         <v>120</v>
       </c>
       <c r="D23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E23" s="3">
         <v>44965</v>
@@ -16086,7 +16082,7 @@
         <v>150</v>
       </c>
       <c r="D24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E24" s="3">
         <v>44965</v>
@@ -16116,7 +16112,7 @@
         <v>151</v>
       </c>
       <c r="D25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E25" s="3">
         <v>44965</v>
@@ -16146,7 +16142,7 @@
         <v>150</v>
       </c>
       <c r="D26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E26" s="3">
         <v>44965</v>
@@ -16176,7 +16172,7 @@
         <v>151</v>
       </c>
       <c r="D27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E27" s="3">
         <v>44965</v>
@@ -16206,7 +16202,7 @@
         <v>151</v>
       </c>
       <c r="D28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E28" s="3">
         <v>44965</v>
@@ -16236,7 +16232,7 @@
         <v>120</v>
       </c>
       <c r="D29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E29" s="3">
         <v>44965</v>
@@ -16266,7 +16262,7 @@
         <v>151</v>
       </c>
       <c r="D30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E30" s="3">
         <v>44965</v>
@@ -16296,7 +16292,7 @@
         <v>120</v>
       </c>
       <c r="D31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E31" s="3">
         <v>44965</v>
@@ -16326,7 +16322,7 @@
         <v>120</v>
       </c>
       <c r="D32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E32" s="3">
         <v>44965</v>
@@ -16356,7 +16352,7 @@
         <v>151</v>
       </c>
       <c r="D33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E33" s="3">
         <v>44965</v>
@@ -16386,7 +16382,7 @@
         <v>150</v>
       </c>
       <c r="D34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E34" s="3">
         <v>44965</v>
@@ -16416,7 +16412,7 @@
         <v>150</v>
       </c>
       <c r="D35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E35" s="3">
         <v>44965</v>
@@ -16459,7 +16455,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Edits for yield1: copes with all NAs in soilmet; corrected time format
</commit_message>
<xml_diff>
--- a/data-raw/skyline_meta-data.xlsx
+++ b/data-raw/skyline_meta-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1950" windowWidth="29040" windowHeight="4125" tabRatio="836" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-28920" yWindow="1950" windowWidth="29040" windowHeight="4125" tabRatio="836" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="2" r:id="rId1"/>
@@ -1407,9 +1407,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1523,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>33</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>253</v>
@@ -1579,7 +1579,7 @@
         <v>33</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="T2" t="s">
         <v>120</v>
@@ -1612,7 +1612,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>33</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>263</v>
@@ -1668,7 +1668,7 @@
         <v>33</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>224</v>
+        <v>270</v>
       </c>
       <c r="T3" t="s">
         <v>120</v>
@@ -2171,7 +2171,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>178</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>178</v>
       </c>
@@ -2317,7 +2317,7 @@
   <autoFilter ref="A1:AC12">
     <filterColumn colId="1">
       <filters>
-        <filter val="diurnal1"/>
+        <filter val="yield1"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2330,7 +2330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -16834,6 +16834,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EF9ABF683E034F89344FAB5B39333E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dee778bbead9c5b03a2ef4f8fda037a0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b04e8096-b088-49dd-9bf5-7c33296d4394" xmlns:ns4="de44e333-4144-40ce-a2c0-3c7c2aff7df8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78a27167cd47c103910f2d57de5b9280" ns3:_="" ns4:_="">
     <xsd:import namespace="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
@@ -17062,36 +17077,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12485A3A-AC12-4EB2-89FF-E5633AE5EFB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33D70FC5-66D0-44F1-ACB8-BD99C781C922}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
-    <ds:schemaRef ds:uri="de44e333-4144-40ce-a2c0-3c7c2aff7df8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17114,9 +17103,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33D70FC5-66D0-44F1-ACB8-BD99C781C922}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12485A3A-AC12-4EB2-89FF-E5633AE5EFB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
+    <ds:schemaRef ds:uri="de44e333-4144-40ce-a2c0-3c7c2aff7df8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Re-added local data file paths in met-data
</commit_message>
<xml_diff>
--- a/data-raw/skyline_meta-data.xlsx
+++ b/data-raw/skyline_meta-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plevy\Documents\skyline\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B03532-DEBA-4131-BD47-406263461911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A9DCCE-4579-4405-A4BA-18783283C458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1368" yWindow="96" windowWidth="17280" windowHeight="6228" tabRatio="836" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1368" yWindow="96" windowWidth="17280" windowHeight="7104" tabRatio="836" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="2" r:id="rId1"/>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2878" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2934" uniqueCount="339">
   <si>
     <t>DOC</t>
   </si>
@@ -1030,15 +1030,6 @@
     <t>2023-09-15</t>
   </si>
   <si>
-    <t>C:\Users\EliApp\Documents\DIVINE WP2 Data\Raw Data\FastVoltage_DAILY</t>
-  </si>
-  <si>
-    <t>C:\Users\EliApp\Documents\DIVINE WP2 Data\Raw Data\CR1000X_DAILY</t>
-  </si>
-  <si>
-    <t>C:\Users\EliApp\Documents\DIVINE WP2 Data\Raw Data\Aeris_DAILY</t>
-  </si>
-  <si>
     <t>t_co2_max</t>
   </si>
   <si>
@@ -1154,6 +1145,42 @@
   </si>
   <si>
     <t>2023-04-03</t>
+  </si>
+  <si>
+    <t>data-raw/raw/EHD/yield1/chi_ghg</t>
+  </si>
+  <si>
+    <t>data-raw/raw/EHD/yield1/chamber_position</t>
+  </si>
+  <si>
+    <t>data-raw/raw/EHD/yield1/soil_met</t>
+  </si>
+  <si>
+    <t>data-raw/raw/EHD/split1/chi_ghg</t>
+  </si>
+  <si>
+    <t>data-raw/raw/EHD/split1/chamber_position</t>
+  </si>
+  <si>
+    <t>data-raw/raw/EHD/biochar1/chamber_position</t>
+  </si>
+  <si>
+    <t>data-raw/raw/EHD/biochar1/chi_ghg</t>
+  </si>
+  <si>
+    <t>data-raw/raw/EHD/split1/soil_met</t>
+  </si>
+  <si>
+    <t>data-raw/raw/EHD/biochar1/soil_met</t>
+  </si>
+  <si>
+    <t>data-raw/raw/HRG/diurnal1/chamber_position</t>
+  </si>
+  <si>
+    <t>data-raw/raw/HRG/diurnal1/chi_ghg</t>
+  </si>
+  <si>
+    <t>data-raw/raw/HRG/diurnal1/soil_met</t>
   </si>
 </sst>
 </file>
@@ -2044,11 +2071,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AG13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E10" sqref="E10"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2128,10 +2157,10 @@
         <v>274</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="S1" s="16" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>166</v>
@@ -2279,13 +2308,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>233</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>284</v>
@@ -2362,16 +2391,16 @@
         <v>9</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>236</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>165</v>
@@ -2380,7 +2409,7 @@
         <v>197</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="I4" s="10">
         <v>12</v>
@@ -2392,7 +2421,7 @@
         <v>205</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="M4" s="10">
         <v>24</v>
@@ -2416,7 +2445,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="14" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="U4" s="21">
         <v>24</v>
@@ -2709,7 +2738,7 @@
         <v>198</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>290</v>
+        <v>337</v>
       </c>
       <c r="I8" s="10">
         <v>1</v>
@@ -2721,7 +2750,7 @@
         <v>245</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>288</v>
+        <v>336</v>
       </c>
       <c r="M8" s="10">
         <v>29</v>
@@ -2745,7 +2774,7 @@
         <v>1</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>289</v>
+        <v>338</v>
       </c>
       <c r="U8" s="21">
         <v>25</v>
@@ -2774,7 +2803,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>235</v>
@@ -2860,10 +2889,10 @@
         <v>235</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>165</v>
@@ -2872,7 +2901,7 @@
         <v>198</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="I10" s="10">
         <v>12</v>
@@ -2884,7 +2913,7 @@
         <v>205</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="M10" s="10">
         <v>21</v>
@@ -2908,7 +2937,7 @@
         <v>0</v>
       </c>
       <c r="T10" s="9" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="U10" s="22">
         <v>40</v>
@@ -2927,6 +2956,270 @@
       </c>
       <c r="Z10" s="14" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="I11" s="10">
+        <v>12</v>
+      </c>
+      <c r="J11" s="10">
+        <v>26</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="M11" s="10">
+        <v>24</v>
+      </c>
+      <c r="N11" s="10">
+        <v>33</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="P11" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>6</v>
+      </c>
+      <c r="R11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S11" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="U11" s="21">
+        <v>24</v>
+      </c>
+      <c r="V11" s="21">
+        <v>33</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="X11" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y11" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z11" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA11" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB11" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC11" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="AD11" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="AE11" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF11" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="I12" s="10">
+        <v>12</v>
+      </c>
+      <c r="J12" s="10">
+        <v>26</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="M12" s="10">
+        <v>24</v>
+      </c>
+      <c r="N12" s="10">
+        <v>38</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="P12" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>6</v>
+      </c>
+      <c r="R12" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S12" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="U12" s="21">
+        <v>24</v>
+      </c>
+      <c r="V12" s="21">
+        <v>38</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="X12" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="Z12" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA12" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="I13" s="10">
+        <v>12</v>
+      </c>
+      <c r="J13" s="10">
+        <v>26</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="M13" s="10">
+        <v>32</v>
+      </c>
+      <c r="N13" s="10">
+        <v>46</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="P13" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>6</v>
+      </c>
+      <c r="R13" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S13" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="T13" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="U13" s="21">
+        <v>32</v>
+      </c>
+      <c r="V13" s="21">
+        <v>46</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="X13" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y13" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="Z13" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="AA13" s="14" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2965,7 +3258,7 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2990,13 +3283,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3007,13 +3300,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3024,13 +3317,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>300</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>303</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3041,10 +3334,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>284</v>
@@ -3058,13 +3351,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>308</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>311</v>
       </c>
       <c r="E7" s="14">
         <v>620</v>
@@ -3075,13 +3368,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E8">
         <v>90</v>
@@ -3143,7 +3436,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>281</v>
@@ -3417,7 +3710,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>119</v>
@@ -3431,7 +3724,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C19" t="s">
         <v>256</v>
@@ -3445,7 +3738,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C20" t="s">
         <v>257</v>
@@ -3459,7 +3752,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C21" t="s">
         <v>258</v>
@@ -3515,7 +3808,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>119</v>
@@ -3529,7 +3822,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>145</v>
@@ -3543,7 +3836,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>146</v>
@@ -15279,7 +15572,7 @@
         <v>9</v>
       </c>
       <c r="B354" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C354" t="s">
         <v>256</v>
@@ -15305,7 +15598,7 @@
         <v>9</v>
       </c>
       <c r="B355" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C355" t="s">
         <v>257</v>
@@ -15331,7 +15624,7 @@
         <v>9</v>
       </c>
       <c r="B356" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C356" t="s">
         <v>258</v>
@@ -15357,7 +15650,7 @@
         <v>9</v>
       </c>
       <c r="B357" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C357" t="s">
         <v>258</v>
@@ -15383,7 +15676,7 @@
         <v>9</v>
       </c>
       <c r="B358" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C358" t="s">
         <v>257</v>
@@ -15409,7 +15702,7 @@
         <v>9</v>
       </c>
       <c r="B359" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C359" t="s">
         <v>256</v>
@@ -15435,7 +15728,7 @@
         <v>9</v>
       </c>
       <c r="B360" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C360" t="s">
         <v>256</v>
@@ -15461,7 +15754,7 @@
         <v>9</v>
       </c>
       <c r="B361" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C361" t="s">
         <v>258</v>
@@ -15487,7 +15780,7 @@
         <v>9</v>
       </c>
       <c r="B362" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C362" t="s">
         <v>257</v>
@@ -15513,7 +15806,7 @@
         <v>9</v>
       </c>
       <c r="B363" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C363" t="s">
         <v>119</v>
@@ -15539,7 +15832,7 @@
         <v>9</v>
       </c>
       <c r="B364" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C364" t="s">
         <v>119</v>
@@ -15565,7 +15858,7 @@
         <v>9</v>
       </c>
       <c r="B365" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C365" t="s">
         <v>256</v>
@@ -15591,7 +15884,7 @@
         <v>9</v>
       </c>
       <c r="B366" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C366" t="s">
         <v>257</v>
@@ -15617,7 +15910,7 @@
         <v>9</v>
       </c>
       <c r="B367" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C367" t="s">
         <v>258</v>
@@ -15643,7 +15936,7 @@
         <v>9</v>
       </c>
       <c r="B368" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C368" t="s">
         <v>257</v>
@@ -15669,7 +15962,7 @@
         <v>9</v>
       </c>
       <c r="B369" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C369" t="s">
         <v>256</v>
@@ -15695,7 +15988,7 @@
         <v>9</v>
       </c>
       <c r="B370" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C370" t="s">
         <v>258</v>
@@ -15721,7 +16014,7 @@
         <v>9</v>
       </c>
       <c r="B371" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C371" t="s">
         <v>257</v>
@@ -15747,7 +16040,7 @@
         <v>9</v>
       </c>
       <c r="B372" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C372" t="s">
         <v>258</v>
@@ -15773,7 +16066,7 @@
         <v>9</v>
       </c>
       <c r="B373" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C373" s="14" t="s">
         <v>256</v>
@@ -15799,7 +16092,7 @@
         <v>9</v>
       </c>
       <c r="B374" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C374" s="14" t="s">
         <v>256</v>
@@ -15825,7 +16118,7 @@
         <v>9</v>
       </c>
       <c r="B375" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C375" s="14" t="s">
         <v>258</v>
@@ -15851,7 +16144,7 @@
         <v>9</v>
       </c>
       <c r="B376" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C376" s="14" t="s">
         <v>257</v>
@@ -15877,7 +16170,7 @@
         <v>9</v>
       </c>
       <c r="B377" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C377" s="14" t="s">
         <v>256</v>
@@ -15903,7 +16196,7 @@
         <v>9</v>
       </c>
       <c r="B378" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C378" s="14" t="s">
         <v>257</v>
@@ -15929,7 +16222,7 @@
         <v>9</v>
       </c>
       <c r="B379" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C379" s="14" t="s">
         <v>258</v>
@@ -15955,7 +16248,7 @@
         <v>9</v>
       </c>
       <c r="B380" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C380" s="14" t="s">
         <v>257</v>
@@ -15981,7 +16274,7 @@
         <v>9</v>
       </c>
       <c r="B381" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C381" s="14" t="s">
         <v>258</v>
@@ -16007,7 +16300,7 @@
         <v>9</v>
       </c>
       <c r="B382" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C382" s="14" t="s">
         <v>256</v>
@@ -16033,7 +16326,7 @@
         <v>9</v>
       </c>
       <c r="B383" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C383" s="14" t="s">
         <v>258</v>
@@ -16059,7 +16352,7 @@
         <v>9</v>
       </c>
       <c r="B384" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C384" s="14" t="s">
         <v>257</v>
@@ -16085,7 +16378,7 @@
         <v>9</v>
       </c>
       <c r="B385" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C385" s="14" t="s">
         <v>256</v>
@@ -16735,7 +17028,7 @@
         <v>9</v>
       </c>
       <c r="B410" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C410" s="14" t="s">
         <v>264</v>
@@ -16761,7 +17054,7 @@
         <v>9</v>
       </c>
       <c r="B411" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C411" s="14" t="s">
         <v>265</v>
@@ -16787,7 +17080,7 @@
         <v>9</v>
       </c>
       <c r="B412" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C412" s="14" t="s">
         <v>263</v>
@@ -16813,7 +17106,7 @@
         <v>9</v>
       </c>
       <c r="B413" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C413" s="14" t="s">
         <v>265</v>
@@ -16839,7 +17132,7 @@
         <v>9</v>
       </c>
       <c r="B414" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C414" s="14" t="s">
         <v>264</v>
@@ -16865,7 +17158,7 @@
         <v>9</v>
       </c>
       <c r="B415" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C415" s="14" t="s">
         <v>263</v>
@@ -16891,7 +17184,7 @@
         <v>9</v>
       </c>
       <c r="B416" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C416" s="14" t="s">
         <v>263</v>
@@ -16917,7 +17210,7 @@
         <v>9</v>
       </c>
       <c r="B417" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C417" s="14" t="s">
         <v>265</v>
@@ -16943,7 +17236,7 @@
         <v>9</v>
       </c>
       <c r="B418" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C418" s="14" t="s">
         <v>264</v>
@@ -16969,7 +17262,7 @@
         <v>9</v>
       </c>
       <c r="B419" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C419" s="14" t="s">
         <v>265</v>
@@ -16995,7 +17288,7 @@
         <v>9</v>
       </c>
       <c r="B420" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C420" s="14" t="s">
         <v>263</v>
@@ -17021,7 +17314,7 @@
         <v>9</v>
       </c>
       <c r="B421" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C421" s="14" t="s">
         <v>264</v>
@@ -17047,7 +17340,7 @@
         <v>9</v>
       </c>
       <c r="B422" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C422" s="14" t="s">
         <v>264</v>
@@ -17073,7 +17366,7 @@
         <v>9</v>
       </c>
       <c r="B423" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C423" s="14" t="s">
         <v>265</v>
@@ -17099,7 +17392,7 @@
         <v>9</v>
       </c>
       <c r="B424" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C424" s="14" t="s">
         <v>263</v>
@@ -17125,7 +17418,7 @@
         <v>9</v>
       </c>
       <c r="B425" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C425" s="14" t="s">
         <v>265</v>
@@ -17151,7 +17444,7 @@
         <v>9</v>
       </c>
       <c r="B426" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C426" s="14" t="s">
         <v>263</v>
@@ -17177,7 +17470,7 @@
         <v>9</v>
       </c>
       <c r="B427" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C427" s="14" t="s">
         <v>264</v>
@@ -17203,7 +17496,7 @@
         <v>9</v>
       </c>
       <c r="B428" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C428" s="14" t="s">
         <v>263</v>
@@ -17229,7 +17522,7 @@
         <v>9</v>
       </c>
       <c r="B429" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C429" s="14" t="s">
         <v>264</v>
@@ -17255,7 +17548,7 @@
         <v>9</v>
       </c>
       <c r="B430" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C430" s="14" t="s">
         <v>265</v>
@@ -17281,7 +17574,7 @@
         <v>9</v>
       </c>
       <c r="B431" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C431" s="14" t="s">
         <v>264</v>
@@ -17307,7 +17600,7 @@
         <v>9</v>
       </c>
       <c r="B432" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C432" s="14" t="s">
         <v>265</v>
@@ -17333,7 +17626,7 @@
         <v>9</v>
       </c>
       <c r="B433" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C433" s="14" t="s">
         <v>263</v>
@@ -17359,7 +17652,7 @@
         <v>9</v>
       </c>
       <c r="B434" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C434" s="14" t="s">
         <v>145</v>
@@ -17385,7 +17678,7 @@
         <v>9</v>
       </c>
       <c r="B435" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C435" s="14" t="s">
         <v>119</v>
@@ -17411,7 +17704,7 @@
         <v>9</v>
       </c>
       <c r="B436" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C436" s="14" t="s">
         <v>146</v>
@@ -17437,7 +17730,7 @@
         <v>9</v>
       </c>
       <c r="B437" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C437" s="14" t="s">
         <v>145</v>
@@ -17463,7 +17756,7 @@
         <v>9</v>
       </c>
       <c r="B438" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C438" s="14" t="s">
         <v>146</v>
@@ -17489,7 +17782,7 @@
         <v>9</v>
       </c>
       <c r="B439" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C439" s="14" t="s">
         <v>119</v>
@@ -17515,7 +17808,7 @@
         <v>9</v>
       </c>
       <c r="B440" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C440" s="14" t="s">
         <v>145</v>
@@ -17541,7 +17834,7 @@
         <v>9</v>
       </c>
       <c r="B441" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C441" s="14" t="s">
         <v>146</v>
@@ -17567,7 +17860,7 @@
         <v>9</v>
       </c>
       <c r="B442" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C442" s="14" t="s">
         <v>119</v>
@@ -17593,7 +17886,7 @@
         <v>9</v>
       </c>
       <c r="B443" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C443" s="14" t="s">
         <v>145</v>
@@ -17619,7 +17912,7 @@
         <v>9</v>
       </c>
       <c r="B444" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C444" s="14" t="s">
         <v>119</v>
@@ -17645,7 +17938,7 @@
         <v>9</v>
       </c>
       <c r="B445" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C445" s="14" t="s">
         <v>146</v>
@@ -17671,7 +17964,7 @@
         <v>9</v>
       </c>
       <c r="B446" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C446" s="14" t="s">
         <v>119</v>
@@ -17697,7 +17990,7 @@
         <v>9</v>
       </c>
       <c r="B447" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C447" s="14" t="s">
         <v>146</v>
@@ -17723,7 +18016,7 @@
         <v>9</v>
       </c>
       <c r="B448" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C448" s="14" t="s">
         <v>145</v>
@@ -17749,7 +18042,7 @@
         <v>9</v>
       </c>
       <c r="B449" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C449" s="14" t="s">
         <v>119</v>
@@ -17775,7 +18068,7 @@
         <v>9</v>
       </c>
       <c r="B450" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C450" s="14" t="s">
         <v>146</v>
@@ -17801,7 +18094,7 @@
         <v>9</v>
       </c>
       <c r="B451" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C451" s="14" t="s">
         <v>145</v>
@@ -17827,7 +18120,7 @@
         <v>9</v>
       </c>
       <c r="B452" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C452" s="14" t="s">
         <v>145</v>
@@ -17853,7 +18146,7 @@
         <v>9</v>
       </c>
       <c r="B453" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C453" s="14" t="s">
         <v>119</v>
@@ -17879,7 +18172,7 @@
         <v>9</v>
       </c>
       <c r="B454" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C454" s="14" t="s">
         <v>146</v>
@@ -17905,7 +18198,7 @@
         <v>9</v>
       </c>
       <c r="B455" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C455" s="14" t="s">
         <v>145</v>
@@ -17931,7 +18224,7 @@
         <v>9</v>
       </c>
       <c r="B456" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C456" s="14" t="s">
         <v>146</v>
@@ -17957,7 +18250,7 @@
         <v>9</v>
       </c>
       <c r="B457" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C457" s="14" t="s">
         <v>119</v>
@@ -17983,7 +18276,7 @@
         <v>9</v>
       </c>
       <c r="B458" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C458" s="14" t="s">
         <v>145</v>
@@ -18009,7 +18302,7 @@
         <v>9</v>
       </c>
       <c r="B459" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C459" s="14" t="s">
         <v>146</v>
@@ -18035,7 +18328,7 @@
         <v>9</v>
       </c>
       <c r="B460" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C460" s="14" t="s">
         <v>119</v>
@@ -18061,7 +18354,7 @@
         <v>9</v>
       </c>
       <c r="B461" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C461" s="14" t="s">
         <v>145</v>
@@ -18087,7 +18380,7 @@
         <v>9</v>
       </c>
       <c r="B462" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C462" s="14" t="s">
         <v>119</v>
@@ -18113,7 +18406,7 @@
         <v>9</v>
       </c>
       <c r="B463" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C463" s="14" t="s">
         <v>146</v>
@@ -18139,7 +18432,7 @@
         <v>9</v>
       </c>
       <c r="B464" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C464" s="14" t="s">
         <v>119</v>
@@ -18165,7 +18458,7 @@
         <v>9</v>
       </c>
       <c r="B465" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C465" s="14" t="s">
         <v>146</v>
@@ -18191,7 +18484,7 @@
         <v>9</v>
       </c>
       <c r="B466" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C466" s="14" t="s">
         <v>145</v>
@@ -18217,7 +18510,7 @@
         <v>9</v>
       </c>
       <c r="B467" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C467" s="14" t="s">
         <v>119</v>
@@ -18243,7 +18536,7 @@
         <v>9</v>
       </c>
       <c r="B468" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C468" s="14" t="s">
         <v>146</v>
@@ -18269,7 +18562,7 @@
         <v>9</v>
       </c>
       <c r="B469" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C469" s="14" t="s">
         <v>145</v>
@@ -18330,7 +18623,7 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>277</v>
@@ -18342,19 +18635,19 @@
         <v>275</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>276</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -18368,7 +18661,7 @@
         <v>279</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E2" s="16">
         <v>0</v>
@@ -18404,7 +18697,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>283</v>
@@ -18440,13 +18733,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E4" s="16">
         <v>0</v>
@@ -18479,13 +18772,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E5" s="16">
         <v>120</v>
@@ -18518,10 +18811,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>284</v>
@@ -18557,13 +18850,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E7" s="16">
         <v>0</v>
@@ -18596,13 +18889,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E8" s="16">
         <v>0</v>
@@ -18758,7 +19051,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>281</v>
@@ -18843,7 +19136,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -18855,7 +19148,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -18863,7 +19156,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C3" s="14">
         <v>2</v>
@@ -18875,7 +19168,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -18883,7 +19176,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C4" s="14">
         <v>3</v>
@@ -18895,7 +19188,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -18903,7 +19196,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C5" s="14">
         <v>4</v>
@@ -18915,7 +19208,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -18923,7 +19216,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C6" s="14">
         <v>5</v>
@@ -18935,7 +19228,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -18943,7 +19236,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C7" s="14">
         <v>6</v>
@@ -18955,7 +19248,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -18963,7 +19256,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C8" s="14">
         <v>7</v>
@@ -18975,7 +19268,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -18983,7 +19276,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C9" s="14">
         <v>8</v>
@@ -18995,7 +19288,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -19003,7 +19296,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C10" s="14">
         <v>9</v>
@@ -19015,7 +19308,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -19023,7 +19316,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C11" s="14">
         <v>10</v>
@@ -19035,7 +19328,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -19043,7 +19336,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C12" s="14">
         <v>11</v>
@@ -19055,7 +19348,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -19063,7 +19356,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C13" s="14">
         <v>12</v>
@@ -19075,7 +19368,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -19083,7 +19376,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C14" s="14">
         <v>13</v>
@@ -19095,7 +19388,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -19103,7 +19396,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C15" s="14">
         <v>14</v>
@@ -19115,7 +19408,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -19123,7 +19416,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C16" s="14">
         <v>15</v>
@@ -19135,7 +19428,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -19143,7 +19436,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C17" s="14">
         <v>16</v>
@@ -19155,7 +19448,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -19163,7 +19456,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C18" s="14">
         <v>17</v>
@@ -19175,7 +19468,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -19183,7 +19476,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C19" s="14">
         <v>18</v>
@@ -19195,7 +19488,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -19203,7 +19496,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C20" s="14">
         <v>19</v>
@@ -19215,7 +19508,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -19223,7 +19516,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C21" s="14">
         <v>20</v>
@@ -19235,7 +19528,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -19243,7 +19536,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C22" s="14">
         <v>21</v>
@@ -19255,7 +19548,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -19263,7 +19556,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C23" s="14">
         <v>22</v>
@@ -19275,7 +19568,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -19283,7 +19576,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C24" s="14">
         <v>23</v>
@@ -19295,7 +19588,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -19303,7 +19596,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C25" s="14">
         <v>24</v>
@@ -19315,7 +19608,7 @@
         <v>44330.999305555553</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -19323,7 +19616,7 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -19335,7 +19628,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F26" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -19343,7 +19636,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C27" s="14">
         <v>2</v>
@@ -19355,7 +19648,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -19363,7 +19656,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C28" s="14">
         <v>3</v>
@@ -19375,7 +19668,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -19383,7 +19676,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C29" s="14">
         <v>4</v>
@@ -19395,7 +19688,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -19403,7 +19696,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C30" s="14">
         <v>5</v>
@@ -19415,7 +19708,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -19423,7 +19716,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C31" s="14">
         <v>6</v>
@@ -19435,7 +19728,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -19443,7 +19736,7 @@
         <v>9</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C32" s="14">
         <v>7</v>
@@ -19455,7 +19748,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -19463,7 +19756,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C33" s="14">
         <v>8</v>
@@ -19475,7 +19768,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -19483,7 +19776,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C34" s="14">
         <v>9</v>
@@ -19495,7 +19788,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -19503,7 +19796,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C35" s="14">
         <v>10</v>
@@ -19515,7 +19808,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -19523,7 +19816,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C36" s="14">
         <v>11</v>
@@ -19535,7 +19828,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -19543,7 +19836,7 @@
         <v>9</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C37" s="14">
         <v>12</v>
@@ -19555,7 +19848,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -19563,7 +19856,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C38" s="14">
         <v>13</v>
@@ -19575,7 +19868,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -19583,7 +19876,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C39" s="14">
         <v>14</v>
@@ -19595,7 +19888,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -19603,7 +19896,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C40" s="14">
         <v>15</v>
@@ -19615,7 +19908,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -19623,7 +19916,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C41" s="14">
         <v>16</v>
@@ -19635,7 +19928,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -19643,7 +19936,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C42" s="14">
         <v>17</v>
@@ -19655,7 +19948,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -19663,7 +19956,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C43" s="14">
         <v>18</v>
@@ -19675,7 +19968,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -19683,7 +19976,7 @@
         <v>9</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C44" s="14">
         <v>19</v>
@@ -19695,7 +19988,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -19703,7 +19996,7 @@
         <v>9</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C45" s="14">
         <v>20</v>
@@ -19715,7 +20008,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -19723,7 +20016,7 @@
         <v>9</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C46" s="14">
         <v>21</v>
@@ -19735,7 +20028,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -19743,7 +20036,7 @@
         <v>9</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C47" s="14">
         <v>22</v>
@@ -19755,7 +20048,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -19763,7 +20056,7 @@
         <v>9</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C48" s="14">
         <v>23</v>
@@ -19775,7 +20068,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -19783,7 +20076,7 @@
         <v>9</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C49" s="14">
         <v>24</v>
@@ -19795,7 +20088,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -19803,7 +20096,7 @@
         <v>9</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C50" s="14">
         <v>25</v>
@@ -19815,7 +20108,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -19823,7 +20116,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C51" s="14">
         <v>26</v>
@@ -19835,7 +20128,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -19843,7 +20136,7 @@
         <v>9</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C52" s="14">
         <v>27</v>
@@ -19855,7 +20148,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -19863,7 +20156,7 @@
         <v>9</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C53" s="14">
         <v>28</v>
@@ -19875,7 +20168,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -19883,7 +20176,7 @@
         <v>9</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C54" s="14">
         <v>29</v>
@@ -19895,7 +20188,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -19903,7 +20196,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C55" s="14">
         <v>30</v>
@@ -19915,7 +20208,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -19923,7 +20216,7 @@
         <v>9</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C56" s="14">
         <v>31</v>
@@ -19935,7 +20228,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -19943,7 +20236,7 @@
         <v>9</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C57" s="14">
         <v>32</v>
@@ -19955,7 +20248,7 @@
         <v>44032.999305555553</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -19975,7 +20268,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F58" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -19995,7 +20288,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -20015,7 +20308,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -20035,7 +20328,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -20055,7 +20348,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -20075,7 +20368,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -20095,7 +20388,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -20115,7 +20408,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -20135,7 +20428,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -20155,7 +20448,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -20175,7 +20468,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F68" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -20195,7 +20488,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F69" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -20215,7 +20508,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -20235,7 +20528,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -20255,7 +20548,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -20275,7 +20568,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -20295,7 +20588,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -20315,7 +20608,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -20335,7 +20628,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -20355,7 +20648,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -20375,7 +20668,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -20395,7 +20688,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -20415,7 +20708,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -20435,7 +20728,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -20455,7 +20748,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -20475,7 +20768,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -20495,7 +20788,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -20515,7 +20808,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -20535,7 +20828,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -20555,7 +20848,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -20575,7 +20868,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -20595,7 +20888,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -20615,7 +20908,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -20635,7 +20928,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -20655,7 +20948,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F92" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -20675,7 +20968,7 @@
         <v>43553.999305555553</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -20695,7 +20988,7 @@
         <v>43636.5</v>
       </c>
       <c r="F94" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -20715,7 +21008,7 @@
         <v>43636.5</v>
       </c>
       <c r="F95" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -20735,7 +21028,7 @@
         <v>43636.5</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -20755,7 +21048,7 @@
         <v>43636.5</v>
       </c>
       <c r="F97" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -20775,7 +21068,7 @@
         <v>43636.5</v>
       </c>
       <c r="F98" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -20795,7 +21088,7 @@
         <v>43636.5</v>
       </c>
       <c r="F99" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -20815,7 +21108,7 @@
         <v>43636.5</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -20835,7 +21128,7 @@
         <v>43636.5</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -20855,7 +21148,7 @@
         <v>43636.5</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -20875,7 +21168,7 @@
         <v>43636.5</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -20895,7 +21188,7 @@
         <v>43636.5</v>
       </c>
       <c r="F104" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -20915,7 +21208,7 @@
         <v>43636.5</v>
       </c>
       <c r="F105" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -20935,7 +21228,7 @@
         <v>43636.5</v>
       </c>
       <c r="F106" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -20955,7 +21248,7 @@
         <v>43636.5</v>
       </c>
       <c r="F107" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -20975,7 +21268,7 @@
         <v>43636.5</v>
       </c>
       <c r="F108" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -20995,7 +21288,7 @@
         <v>43636.5</v>
       </c>
       <c r="F109" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -21015,7 +21308,7 @@
         <v>43636.5</v>
       </c>
       <c r="F110" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -21035,7 +21328,7 @@
         <v>43636.5</v>
       </c>
       <c r="F111" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -21055,7 +21348,7 @@
         <v>43636.5</v>
       </c>
       <c r="F112" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -21075,7 +21368,7 @@
         <v>43636.5</v>
       </c>
       <c r="F113" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -21095,7 +21388,7 @@
         <v>43636.5</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -21115,7 +21408,7 @@
         <v>43636.5</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -21135,7 +21428,7 @@
         <v>43636.5</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -21155,7 +21448,7 @@
         <v>43636.5</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -21175,7 +21468,7 @@
         <v>43636.5</v>
       </c>
       <c r="F118" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -21195,7 +21488,7 @@
         <v>43636.5</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -21215,7 +21508,7 @@
         <v>43636.5</v>
       </c>
       <c r="F120" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -21235,7 +21528,7 @@
         <v>43636.5</v>
       </c>
       <c r="F121" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -21255,7 +21548,7 @@
         <v>43636.5</v>
       </c>
       <c r="F122" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -21275,7 +21568,7 @@
         <v>43636.5</v>
       </c>
       <c r="F123" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -21295,7 +21588,7 @@
         <v>43636.5</v>
       </c>
       <c r="F124" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -21315,7 +21608,7 @@
         <v>43636.5</v>
       </c>
       <c r="F125" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -21335,7 +21628,7 @@
         <v>43636.5</v>
       </c>
       <c r="F126" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -21355,7 +21648,7 @@
         <v>43636.5</v>
       </c>
       <c r="F127" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -21375,7 +21668,7 @@
         <v>43636.5</v>
       </c>
       <c r="F128" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -21395,12 +21688,12 @@
         <v>43636.5</v>
       </c>
       <c r="F129" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B130" t="s">
         <v>158</v>
@@ -21415,12 +21708,12 @@
         <v>45111.916666666664</v>
       </c>
       <c r="F130" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B131" s="14" t="s">
         <v>158</v>
@@ -21435,12 +21728,12 @@
         <v>45129.708333333336</v>
       </c>
       <c r="F131" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B132" s="14" t="s">
         <v>158</v>
@@ -21457,7 +21750,7 @@
     </row>
     <row r="133" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B133" s="14" t="s">
         <v>158</v>
@@ -21474,7 +21767,7 @@
     </row>
     <row r="134" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B134" s="14" t="s">
         <v>158</v>
@@ -21491,7 +21784,7 @@
     </row>
     <row r="135" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B135" s="14" t="s">
         <v>158</v>
@@ -21508,7 +21801,7 @@
     </row>
     <row r="136" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B136" s="14" t="s">
         <v>158</v>
@@ -21525,7 +21818,7 @@
     </row>
     <row r="137" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B137" s="14" t="s">
         <v>158</v>
@@ -21542,7 +21835,7 @@
     </row>
     <row r="138" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B138" s="14" t="s">
         <v>158</v>
@@ -21559,7 +21852,7 @@
     </row>
     <row r="139" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B139" s="14" t="s">
         <v>158</v>
@@ -21576,7 +21869,7 @@
     </row>
     <row r="140" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B140" s="14" t="s">
         <v>158</v>
@@ -21593,7 +21886,7 @@
     </row>
     <row r="141" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B141" s="14" t="s">
         <v>158</v>
@@ -21610,7 +21903,7 @@
     </row>
     <row r="142" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B142" s="14" t="s">
         <v>158</v>
@@ -21627,7 +21920,7 @@
     </row>
     <row r="143" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B143" s="14" t="s">
         <v>158</v>
@@ -21644,7 +21937,7 @@
     </row>
     <row r="144" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B144" s="14" t="s">
         <v>158</v>
@@ -21661,7 +21954,7 @@
     </row>
     <row r="145" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B145" s="14" t="s">
         <v>158</v>
@@ -21678,7 +21971,7 @@
     </row>
     <row r="146" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B146" s="14" t="s">
         <v>158</v>
@@ -21695,7 +21988,7 @@
     </row>
     <row r="147" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B147" s="14" t="s">
         <v>158</v>
@@ -21712,7 +22005,7 @@
     </row>
     <row r="148" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B148" s="14" t="s">
         <v>158</v>
@@ -21729,7 +22022,7 @@
     </row>
     <row r="149" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B149" s="14" t="s">
         <v>158</v>
@@ -21746,7 +22039,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B150" s="14" t="s">
         <v>158</v>
@@ -21763,7 +22056,7 @@
     </row>
     <row r="151" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B151" s="14" t="s">
         <v>158</v>
@@ -21780,7 +22073,7 @@
     </row>
     <row r="152" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B152" s="14" t="s">
         <v>158</v>
@@ -21797,7 +22090,7 @@
     </row>
     <row r="153" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B153" s="14" t="s">
         <v>158</v>
@@ -21814,7 +22107,7 @@
     </row>
     <row r="154" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B154" s="14" t="s">
         <v>158</v>
@@ -21831,7 +22124,7 @@
     </row>
     <row r="155" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B155" s="14" t="s">
         <v>158</v>
@@ -21848,7 +22141,7 @@
     </row>
     <row r="156" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B156" s="14" t="s">
         <v>158</v>
@@ -21865,7 +22158,7 @@
     </row>
     <row r="157" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B157" s="14" t="s">
         <v>158</v>
@@ -21882,7 +22175,7 @@
     </row>
     <row r="158" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B158" s="14" t="s">
         <v>158</v>
@@ -21899,7 +22192,7 @@
     </row>
     <row r="159" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B159" s="14" t="s">
         <v>158</v>
@@ -21916,7 +22209,7 @@
     </row>
     <row r="160" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B160" s="14" t="s">
         <v>158</v>
@@ -21933,7 +22226,7 @@
     </row>
     <row r="161" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B161" s="14" t="s">
         <v>158</v>
@@ -21950,7 +22243,7 @@
     </row>
     <row r="162" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B162" s="14" t="s">
         <v>158</v>
@@ -21967,7 +22260,7 @@
     </row>
     <row r="163" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B163" s="14" t="s">
         <v>158</v>
@@ -21984,7 +22277,7 @@
     </row>
     <row r="164" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B164" s="14" t="s">
         <v>158</v>
@@ -22001,7 +22294,7 @@
     </row>
     <row r="165" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B165" s="14" t="s">
         <v>158</v>
@@ -22018,7 +22311,7 @@
     </row>
     <row r="166" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B166" s="14" t="s">
         <v>158</v>
@@ -22035,7 +22328,7 @@
     </row>
     <row r="167" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B167" s="14" t="s">
         <v>158</v>
@@ -22052,7 +22345,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B168" s="14" t="s">
         <v>158</v>
@@ -22069,7 +22362,7 @@
     </row>
     <row r="169" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B169" s="14" t="s">
         <v>158</v>
@@ -22086,7 +22379,7 @@
     </row>
     <row r="170" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B170" s="14" t="s">
         <v>158</v>
@@ -22103,7 +22396,7 @@
     </row>
     <row r="171" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A171" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B171" s="14" t="s">
         <v>158</v>
@@ -22120,7 +22413,7 @@
     </row>
     <row r="172" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B172" s="14" t="s">
         <v>158</v>
@@ -22137,7 +22430,7 @@
     </row>
     <row r="173" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B173" s="14" t="s">
         <v>158</v>
@@ -22154,7 +22447,7 @@
     </row>
     <row r="174" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B174" s="14" t="s">
         <v>158</v>
@@ -22171,7 +22464,7 @@
     </row>
     <row r="175" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B175" s="14" t="s">
         <v>158</v>
@@ -22188,7 +22481,7 @@
     </row>
     <row r="176" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B176" s="14" t="s">
         <v>158</v>
@@ -22205,7 +22498,7 @@
     </row>
     <row r="177" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B177" s="14" t="s">
         <v>158</v>
@@ -22222,7 +22515,7 @@
     </row>
     <row r="178" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B178" s="14" t="s">
         <v>158</v>
@@ -22239,7 +22532,7 @@
     </row>
     <row r="179" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B179" s="14" t="s">
         <v>158</v>
@@ -22256,7 +22549,7 @@
     </row>
     <row r="180" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B180" s="14" t="s">
         <v>158</v>
@@ -22273,7 +22566,7 @@
     </row>
     <row r="181" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A181" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B181" s="14" t="s">
         <v>158</v>
@@ -22290,7 +22583,7 @@
     </row>
     <row r="182" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B182" s="14" t="s">
         <v>158</v>
@@ -22307,7 +22600,7 @@
     </row>
     <row r="183" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B183" s="14" t="s">
         <v>158</v>
@@ -22324,7 +22617,7 @@
     </row>
     <row r="184" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B184" s="14" t="s">
         <v>158</v>
@@ -22341,7 +22634,7 @@
     </row>
     <row r="185" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B185" s="14" t="s">
         <v>158</v>
@@ -22358,7 +22651,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B186" s="14" t="s">
         <v>158</v>
@@ -22375,7 +22668,7 @@
     </row>
     <row r="187" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B187" s="14" t="s">
         <v>158</v>
@@ -22392,7 +22685,7 @@
     </row>
     <row r="188" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B188" s="14" t="s">
         <v>158</v>
@@ -22409,7 +22702,7 @@
     </row>
     <row r="189" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B189" s="14" t="s">
         <v>158</v>
@@ -22426,7 +22719,7 @@
     </row>
     <row r="190" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B190" s="14" t="s">
         <v>158</v>
@@ -22443,7 +22736,7 @@
     </row>
     <row r="191" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B191" s="14" t="s">
         <v>158</v>
@@ -22460,7 +22753,7 @@
     </row>
     <row r="192" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B192" s="14" t="s">
         <v>158</v>
@@ -22477,7 +22770,7 @@
     </row>
     <row r="193" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B193" s="14" t="s">
         <v>158</v>
@@ -22494,7 +22787,7 @@
     </row>
     <row r="194" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B194" s="14" t="s">
         <v>158</v>
@@ -22511,7 +22804,7 @@
     </row>
     <row r="195" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A195" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B195" s="14" t="s">
         <v>158</v>
@@ -22528,7 +22821,7 @@
     </row>
     <row r="196" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B196" s="14" t="s">
         <v>158</v>
@@ -22545,7 +22838,7 @@
     </row>
     <row r="197" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B197" s="14" t="s">
         <v>158</v>
@@ -22562,7 +22855,7 @@
     </row>
     <row r="198" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B198" s="14" t="s">
         <v>158</v>
@@ -22579,7 +22872,7 @@
     </row>
     <row r="199" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B199" s="14" t="s">
         <v>158</v>
@@ -22596,7 +22889,7 @@
     </row>
     <row r="200" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B200" s="14" t="s">
         <v>158</v>
@@ -22613,7 +22906,7 @@
     </row>
     <row r="201" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B201" s="14" t="s">
         <v>158</v>
@@ -22630,7 +22923,7 @@
     </row>
     <row r="202" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B202" s="14" t="s">
         <v>158</v>
@@ -22647,7 +22940,7 @@
     </row>
     <row r="203" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B203" s="14" t="s">
         <v>158</v>
@@ -22664,7 +22957,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B204" s="14" t="s">
         <v>158</v>
@@ -22681,7 +22974,7 @@
     </row>
     <row r="205" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B205" s="14" t="s">
         <v>158</v>
@@ -22698,7 +22991,7 @@
     </row>
     <row r="206" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B206" s="14" t="s">
         <v>158</v>
@@ -22715,7 +23008,7 @@
     </row>
     <row r="207" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B207" s="14" t="s">
         <v>158</v>
@@ -22732,7 +23025,7 @@
     </row>
     <row r="208" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B208" s="14" t="s">
         <v>158</v>
@@ -22749,7 +23042,7 @@
     </row>
     <row r="209" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B209" s="14" t="s">
         <v>158</v>
@@ -22766,7 +23059,7 @@
     </row>
     <row r="210" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B210" s="14" t="s">
         <v>158</v>
@@ -22783,7 +23076,7 @@
     </row>
     <row r="211" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B211" s="14" t="s">
         <v>158</v>
@@ -22800,7 +23093,7 @@
     </row>
     <row r="212" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B212" s="14" t="s">
         <v>158</v>
@@ -22817,7 +23110,7 @@
     </row>
     <row r="213" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B213" s="14" t="s">
         <v>158</v>
@@ -22834,7 +23127,7 @@
     </row>
     <row r="214" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B214" s="14" t="s">
         <v>158</v>
@@ -22851,7 +23144,7 @@
     </row>
     <row r="215" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B215" s="14" t="s">
         <v>158</v>
@@ -22868,7 +23161,7 @@
     </row>
     <row r="216" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B216" s="14" t="s">
         <v>158</v>
@@ -22885,7 +23178,7 @@
     </row>
     <row r="217" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B217" s="14" t="s">
         <v>158</v>
@@ -22902,7 +23195,7 @@
     </row>
     <row r="218" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B218" s="14" t="s">
         <v>158</v>
@@ -22919,7 +23212,7 @@
     </row>
     <row r="219" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B219" s="14" t="s">
         <v>158</v>
@@ -22936,7 +23229,7 @@
     </row>
     <row r="220" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B220" s="14" t="s">
         <v>158</v>
@@ -22953,7 +23246,7 @@
     </row>
     <row r="221" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A221" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B221" s="14" t="s">
         <v>158</v>

</xml_diff>

<commit_message>
Removed shortening of CO2 data
</commit_message>
<xml_diff>
--- a/data-raw/skyline_meta-data.xlsx
+++ b/data-raw/skyline_meta-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plevy\AppData\Local\Temp\scp50647\gpfs01\home\plevy\skyline\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3F5E9F-21A7-4B5B-9145-A1F63BD1CD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C1A7F0-D0D3-44D8-908E-5F0B86BED276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="6885" windowWidth="18510" windowHeight="6930" tabRatio="662" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4104" yWindow="4116" windowWidth="18516" windowHeight="6936" tabRatio="662" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="2" r:id="rId1"/>
@@ -2040,7 +2040,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16436,8 +16436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F766238-C12B-4ECD-BCE0-551F5AD99049}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed deadband detection to use co2
</commit_message>
<xml_diff>
--- a/data-raw/skyline_meta-data.xlsx
+++ b/data-raw/skyline_meta-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plevy\AppData\Local\Temp\scp50647\gpfs01\home\plevy\skyline\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plevy\AppData\Local\Temp\scp09372\gpfs01\home\plevy\skyline\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C1A7F0-D0D3-44D8-908E-5F0B86BED276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AF18B9-7844-4DC5-93CA-AC03E04100B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4104" yWindow="4116" windowWidth="18516" windowHeight="6936" tabRatio="662" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="3675" windowWidth="21600" windowHeight="11385" tabRatio="662" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="2" r:id="rId1"/>
@@ -16436,8 +16436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F766238-C12B-4ECD-BCE0-551F5AD99049}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16522,7 +16522,7 @@
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="16">
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="L2" s="17" t="b">
         <v>1</v>
@@ -16561,7 +16561,7 @@
       </c>
       <c r="J3" s="16"/>
       <c r="K3" s="16">
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="L3" s="17" t="b">
         <v>1</v>
@@ -16600,7 +16600,7 @@
       </c>
       <c r="J4" s="16"/>
       <c r="K4" s="16">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="L4" s="17" t="b">
         <v>1</v>
@@ -16639,7 +16639,7 @@
       </c>
       <c r="J5" s="16"/>
       <c r="K5" s="16">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="L5" s="17" t="b">
         <v>1</v>
@@ -16678,7 +16678,7 @@
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="16">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="17" t="b">
         <v>1</v>
@@ -16717,7 +16717,7 @@
       </c>
       <c r="J7" s="16"/>
       <c r="K7" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" s="17" t="b">
         <v>1</v>
@@ -16758,7 +16758,7 @@
         <v>200</v>
       </c>
       <c r="K8" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" s="17" t="b">
         <v>1</v>
@@ -16797,7 +16797,7 @@
       </c>
       <c r="J9" s="16"/>
       <c r="K9" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" s="17" t="b">
         <v>1</v>
@@ -16838,7 +16838,7 @@
         <v>200</v>
       </c>
       <c r="K10" s="16">
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="L10" s="17" t="b">
         <v>0</v>
@@ -16879,7 +16879,7 @@
         <v>120</v>
       </c>
       <c r="K11" s="16">
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="L11" s="17" t="b">
         <v>0</v>
@@ -16905,7 +16905,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="16">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="G12" s="16">
         <v>45</v>
@@ -16920,7 +16920,7 @@
         <v>200</v>
       </c>
       <c r="K12" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="17" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added Shipton DIVINE expt
</commit_message>
<xml_diff>
--- a/data-raw/skyline_meta-data.xlsx
+++ b/data-raw/skyline_meta-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plevy\AppData\Local\Temp\scp19940\gws\nopw\j04\ceh_generic\plevy\skyline\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plevy\AppData\Local\Temp\scp47960\gws\nopw\j04\ceh_generic\plevy\skyline\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7226A6-884B-4613-97CE-DD09C6D579FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C447E3A9-E816-4799-8EF5-096BBA05B3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="662" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" tabRatio="662" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="2" r:id="rId1"/>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3225" uniqueCount="392">
   <si>
     <t>DOC</t>
   </si>
@@ -1287,6 +1287,51 @@
   </si>
   <si>
     <t>shading1</t>
+  </si>
+  <si>
+    <t>SHP</t>
+  </si>
+  <si>
+    <t>Shipton</t>
+  </si>
+  <si>
+    <t>divine1</t>
+  </si>
+  <si>
+    <t>DIVINE 1</t>
+  </si>
+  <si>
+    <t>data-raw/raw/SHP/divine1/chi_ghg</t>
+  </si>
+  <si>
+    <t>data-raw/raw/SHP/divine1/chamber_position</t>
+  </si>
+  <si>
+    <t>data-raw/raw/SHP/divine1/soil_met</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>2023-03-17</t>
+  </si>
+  <si>
+    <t>2023-07-24</t>
+  </si>
+  <si>
+    <t>Los Gatos</t>
+  </si>
+  <si>
+    <t>block2</t>
+  </si>
+  <si>
+    <t>block1</t>
+  </si>
+  <si>
+    <t>Dummy1</t>
+  </si>
+  <si>
+    <t>Dummy2</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1383,6 +1428,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1680,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1791,6 +1839,20 @@
       </c>
       <c r="D5">
         <v>51.844724999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2183,13 +2245,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2944,6 +3006,80 @@
         <v>320</v>
       </c>
     </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>377</v>
+      </c>
+      <c r="B9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="I9" s="9">
+        <v>8</v>
+      </c>
+      <c r="J9" s="9">
+        <v>17</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="M9" s="9">
+        <v>1</v>
+      </c>
+      <c r="N9" s="9">
+        <v>10</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="P9" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="R9" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="U9" s="9">
+        <v>1</v>
+      </c>
+      <c r="V9" s="9">
+        <v>10</v>
+      </c>
+      <c r="W9" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="X9" s="18">
+        <v>5</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH7">
     <sortCondition ref="A2:A7"/>
@@ -2959,10 +3095,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D30447-6404-4F75-9FF7-A1D31B37D762}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3175,6 +3311,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>377</v>
+      </c>
+      <c r="B13" t="s">
+        <v>379</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3182,10 +3335,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A10" zoomScale="81" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3658,6 +3811,40 @@
         <v>345</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>377</v>
+      </c>
+      <c r="B29" t="s">
+        <v>379</v>
+      </c>
+      <c r="C29" t="s">
+        <v>389</v>
+      </c>
+      <c r="D29" t="s">
+        <v>390</v>
+      </c>
+      <c r="E29" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>377</v>
+      </c>
+      <c r="B30" t="s">
+        <v>379</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D30" t="s">
+        <v>391</v>
+      </c>
+      <c r="E30" t="s">
+        <v>332</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3666,11 +3853,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:S108"/>
+  <dimension ref="A1:S109"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7687,6 +7874,35 @@
         <v>355</v>
       </c>
     </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>377</v>
+      </c>
+      <c r="B109" t="s">
+        <v>379</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F109" s="3">
+        <v>45047</v>
+      </c>
+      <c r="G109" s="3">
+        <v>45047</v>
+      </c>
+      <c r="I109">
+        <v>100</v>
+      </c>
+      <c r="J109" t="s">
+        <v>384</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7696,11 +7912,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J445"/>
+  <dimension ref="A1:J461"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B151" sqref="B151"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A441" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C454" sqref="C454:C461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19289,6 +19505,422 @@
         <v>45565</v>
       </c>
     </row>
+    <row r="446" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A446" t="s">
+        <v>377</v>
+      </c>
+      <c r="B446" t="s">
+        <v>379</v>
+      </c>
+      <c r="C446" t="s">
+        <v>389</v>
+      </c>
+      <c r="D446">
+        <v>1</v>
+      </c>
+      <c r="E446">
+        <v>0.113354</v>
+      </c>
+      <c r="F446">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G446" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H446" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="447" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A447" t="s">
+        <v>377</v>
+      </c>
+      <c r="B447" t="s">
+        <v>379</v>
+      </c>
+      <c r="C447" t="s">
+        <v>389</v>
+      </c>
+      <c r="D447">
+        <v>2</v>
+      </c>
+      <c r="E447">
+        <v>0.113354</v>
+      </c>
+      <c r="F447">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G447" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H447" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="448" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A448" t="s">
+        <v>377</v>
+      </c>
+      <c r="B448" t="s">
+        <v>379</v>
+      </c>
+      <c r="C448" t="s">
+        <v>389</v>
+      </c>
+      <c r="D448">
+        <v>3</v>
+      </c>
+      <c r="E448">
+        <v>0.113354</v>
+      </c>
+      <c r="F448">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G448" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H448" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="449" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A449" t="s">
+        <v>377</v>
+      </c>
+      <c r="B449" t="s">
+        <v>379</v>
+      </c>
+      <c r="C449" t="s">
+        <v>389</v>
+      </c>
+      <c r="D449">
+        <v>4</v>
+      </c>
+      <c r="E449">
+        <v>0.113354</v>
+      </c>
+      <c r="F449">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G449" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H449" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="450" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A450" t="s">
+        <v>377</v>
+      </c>
+      <c r="B450" t="s">
+        <v>379</v>
+      </c>
+      <c r="C450" t="s">
+        <v>389</v>
+      </c>
+      <c r="D450">
+        <v>5</v>
+      </c>
+      <c r="E450">
+        <v>0.113354</v>
+      </c>
+      <c r="F450">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G450" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H450" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="451" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A451" t="s">
+        <v>377</v>
+      </c>
+      <c r="B451" t="s">
+        <v>379</v>
+      </c>
+      <c r="C451" t="s">
+        <v>389</v>
+      </c>
+      <c r="D451">
+        <v>6</v>
+      </c>
+      <c r="E451">
+        <v>0.113354</v>
+      </c>
+      <c r="F451">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G451" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H451" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="452" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A452" t="s">
+        <v>377</v>
+      </c>
+      <c r="B452" t="s">
+        <v>379</v>
+      </c>
+      <c r="C452" t="s">
+        <v>389</v>
+      </c>
+      <c r="D452">
+        <v>7</v>
+      </c>
+      <c r="E452">
+        <v>0.113354</v>
+      </c>
+      <c r="F452">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G452" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H452" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="453" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A453" t="s">
+        <v>377</v>
+      </c>
+      <c r="B453" t="s">
+        <v>379</v>
+      </c>
+      <c r="C453" t="s">
+        <v>389</v>
+      </c>
+      <c r="D453">
+        <v>8</v>
+      </c>
+      <c r="E453">
+        <v>0.113354</v>
+      </c>
+      <c r="F453">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G453" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H453" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="454" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A454" t="s">
+        <v>377</v>
+      </c>
+      <c r="B454" t="s">
+        <v>379</v>
+      </c>
+      <c r="C454" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D454">
+        <v>9</v>
+      </c>
+      <c r="E454">
+        <v>0.113354</v>
+      </c>
+      <c r="F454">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G454" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H454" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="455" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
+        <v>377</v>
+      </c>
+      <c r="B455" t="s">
+        <v>379</v>
+      </c>
+      <c r="C455" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D455">
+        <v>10</v>
+      </c>
+      <c r="E455">
+        <v>0.113354</v>
+      </c>
+      <c r="F455">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G455" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H455" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="456" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A456" t="s">
+        <v>377</v>
+      </c>
+      <c r="B456" t="s">
+        <v>379</v>
+      </c>
+      <c r="C456" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D456">
+        <v>11</v>
+      </c>
+      <c r="E456">
+        <v>0.113354</v>
+      </c>
+      <c r="F456">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G456" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H456" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="457" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A457" t="s">
+        <v>377</v>
+      </c>
+      <c r="B457" t="s">
+        <v>379</v>
+      </c>
+      <c r="C457" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D457">
+        <v>12</v>
+      </c>
+      <c r="E457">
+        <v>0.113354</v>
+      </c>
+      <c r="F457">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G457" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H457" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="458" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A458" t="s">
+        <v>377</v>
+      </c>
+      <c r="B458" t="s">
+        <v>379</v>
+      </c>
+      <c r="C458" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D458">
+        <v>13</v>
+      </c>
+      <c r="E458">
+        <v>0.113354</v>
+      </c>
+      <c r="F458">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G458" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H458" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="459" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A459" t="s">
+        <v>377</v>
+      </c>
+      <c r="B459" t="s">
+        <v>379</v>
+      </c>
+      <c r="C459" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D459">
+        <v>14</v>
+      </c>
+      <c r="E459">
+        <v>0.113354</v>
+      </c>
+      <c r="F459">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G459" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H459" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="460" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A460" t="s">
+        <v>377</v>
+      </c>
+      <c r="B460" t="s">
+        <v>379</v>
+      </c>
+      <c r="C460" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D460">
+        <v>15</v>
+      </c>
+      <c r="E460">
+        <v>0.113354</v>
+      </c>
+      <c r="F460">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G460" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H460" s="3">
+        <v>45131</v>
+      </c>
+    </row>
+    <row r="461" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A461" t="s">
+        <v>377</v>
+      </c>
+      <c r="B461" t="s">
+        <v>379</v>
+      </c>
+      <c r="C461" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D461">
+        <v>16</v>
+      </c>
+      <c r="E461">
+        <v>0.113354</v>
+      </c>
+      <c r="F461">
+        <v>8.924087E-2</v>
+      </c>
+      <c r="G461" s="3">
+        <v>45002</v>
+      </c>
+      <c r="H461" s="3">
+        <v>45131</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19298,10 +19930,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F766238-C12B-4ECD-BCE0-551F5AD99049}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19866,6 +20498,44 @@
         <v>0</v>
       </c>
       <c r="M14" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>377</v>
+      </c>
+      <c r="B15" t="s">
+        <v>379</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0</v>
+      </c>
+      <c r="F15" s="12">
+        <v>100</v>
+      </c>
+      <c r="G15" s="12">
+        <v>60</v>
+      </c>
+      <c r="H15" s="12">
+        <v>360</v>
+      </c>
+      <c r="I15" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="12">
+        <v>2</v>
+      </c>
+      <c r="L15" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -24055,7 +24725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -24670,12 +25340,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EF9ABF683E034F89344FAB5B39333E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dee778bbead9c5b03a2ef4f8fda037a0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b04e8096-b088-49dd-9bf5-7c33296d4394" xmlns:ns4="de44e333-4144-40ce-a2c0-3c7c2aff7df8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78a27167cd47c103910f2d57de5b9280" ns3:_="" ns4:_="">
     <xsd:import namespace="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
@@ -24904,6 +25568,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33D70FC5-66D0-44F1-ACB8-BD99C781C922}">
   <ds:schemaRefs>
@@ -24913,23 +25583,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1591EC7B-C469-4BBA-B7FD-C66217A363C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="de44e333-4144-40ce-a2c0-3c7c2aff7df8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12485A3A-AC12-4EB2-89FF-E5633AE5EFB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24946,4 +25599,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1591EC7B-C469-4BBA-B7FD-C66217A363C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="de44e333-4144-40ce-a2c0-3c7c2aff7df8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b04e8096-b088-49dd-9bf5-7c33296d4394"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>